<commit_message>
Delete invalid tests from login and register tab.
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="117">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -111,6 +111,9 @@
   <si>
     <t xml:space="preserve">Not need valid email for registration. 
 Generate email account random string.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Playwright tool.</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -242,55 +245,16 @@
     <t xml:space="preserve">001-14</t>
   </si>
   <si>
-    <t xml:space="preserve">Register with changed email.</t>
+    <t xml:space="preserve">Register user confirm password not matching password</t>
   </si>
   <si>
-    <t xml:space="preserve">User is registered with changed email.</t>
+    <t xml:space="preserve">User shouldn’t able to register without the Password and Confirm password fields are matching. Error message.</t>
   </si>
   <si>
     <t xml:space="preserve">001-15</t>
   </si>
   <si>
-    <t xml:space="preserve">Register with invalid changed mail.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User shouldn't able to register with invalid change mail. Error message.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">001-16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Register without select date of birth day.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User shouldn't able to register without selecting date of birth day. Error message.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">001-17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Register without select date of birth month.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User shouldn't able to register without selecting date of birth month. Error message.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">001-18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Register without select date of birth year.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should able to register without selecting date of birth year. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">001-19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Register without select.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should able to register without selecting date. Error message.</t>
+    <t xml:space="preserve">Register user Password field change after fill Password and Confirm password field.</t>
   </si>
   <si>
     <t xml:space="preserve">Buy product</t>
@@ -310,9 +274,6 @@
 Product not in the stock.</t>
   </si>
   <si>
-    <t xml:space="preserve">Cypress tool.</t>
-  </si>
-  <si>
     <t xml:space="preserve">002-01</t>
   </si>
   <si>
@@ -320,15 +281,6 @@
   </si>
   <si>
     <t xml:space="preserve">User should buy single product.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User can buy single product.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
   </si>
   <si>
     <t xml:space="preserve">002-02</t>
@@ -340,16 +292,10 @@
     <t xml:space="preserve">User should buy multiple products.</t>
   </si>
   <si>
-    <t xml:space="preserve">User can buy multiple product.</t>
-  </si>
-  <si>
     <t xml:space="preserve">002-03</t>
   </si>
   <si>
     <t xml:space="preserve">Buy multiple products different product.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User can buy multiple quantity from multiple product.</t>
   </si>
   <si>
     <t xml:space="preserve">002-04</t>
@@ -361,9 +307,6 @@
     <t xml:space="preserve">Cart should be empty.</t>
   </si>
   <si>
-    <t xml:space="preserve">Cart empty after user deleting item from it.</t>
-  </si>
-  <si>
     <t xml:space="preserve">002-05</t>
   </si>
   <si>
@@ -373,9 +316,6 @@
     <t xml:space="preserve">Only that product is missing which is removed.</t>
   </si>
   <si>
-    <t xml:space="preserve">Cart has one product after other product is deleted.</t>
-  </si>
-  <si>
     <t xml:space="preserve">002-06</t>
   </si>
   <si>
@@ -383,9 +323,6 @@
   </si>
   <si>
     <t xml:space="preserve">More product in the cart.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cart has increased the amount size.</t>
   </si>
   <si>
     <t xml:space="preserve">002-07</t>
@@ -1212,9 +1149,9 @@
   <dimension ref="A1:EZ899"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1514,7 +1451,9 @@
         <v>23</v>
       </c>
       <c r="G8" s="5"/>
-      <c r="H8" s="21"/>
+      <c r="H8" s="21" t="s">
+        <v>24</v>
+      </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -1532,42 +1471,42 @@
     <row r="10" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="18"/>
       <c r="B10" s="23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="25" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H10" s="26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I10" s="26"/>
       <c r="J10" s="26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="33"/>
@@ -1578,14 +1517,14 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F12" s="32"/>
       <c r="G12" s="33"/>
@@ -1596,14 +1535,14 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F13" s="32"/>
       <c r="G13" s="33"/>
@@ -1614,14 +1553,14 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="33"/>
@@ -1632,14 +1571,14 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F15" s="32"/>
       <c r="G15" s="33"/>
@@ -1650,14 +1589,14 @@
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F16" s="32"/>
       <c r="G16" s="33"/>
@@ -1668,14 +1607,14 @@
     <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="33"/>
@@ -1686,14 +1625,14 @@
     <row r="18" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F18" s="32"/>
       <c r="G18" s="33"/>
@@ -1704,38 +1643,38 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
     </row>
     <row r="20" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -1743,14 +1682,14 @@
     <row r="21" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="33"/>
@@ -1761,14 +1700,14 @@
     <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="33"/>
@@ -1779,14 +1718,14 @@
     <row r="23" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="33"/>
@@ -1794,17 +1733,17 @@
       <c r="I23" s="32"/>
       <c r="J23" s="32"/>
     </row>
-    <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="18"/>
+    <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0"/>
       <c r="B24" s="30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="33"/>
@@ -1812,17 +1751,17 @@
       <c r="I24" s="32"/>
       <c r="J24" s="32"/>
     </row>
-    <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="18"/>
+    <row r="25" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0"/>
       <c r="B25" s="30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="33"/>
@@ -1831,76 +1770,48 @@
       <c r="J25" s="32"/>
     </row>
     <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="18"/>
-      <c r="B26" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
+      <c r="A26" s="0"/>
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+      <c r="D26" s="0"/>
+      <c r="E26" s="0"/>
+      <c r="F26" s="0"/>
+      <c r="G26" s="0"/>
+      <c r="H26" s="0"/>
+      <c r="I26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="18"/>
-      <c r="B27" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="F27" s="32"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
+      <c r="A27" s="0"/>
+      <c r="B27" s="0"/>
+      <c r="C27" s="0"/>
+      <c r="D27" s="0"/>
+      <c r="E27" s="0"/>
+      <c r="F27" s="0"/>
+      <c r="G27" s="0"/>
+      <c r="H27" s="0"/>
+      <c r="I27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="18"/>
-      <c r="B28" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
+      <c r="C28" s="0"/>
+      <c r="D28" s="0"/>
+      <c r="E28" s="0"/>
+      <c r="F28" s="0"/>
+      <c r="G28" s="0"/>
+      <c r="H28" s="0"/>
+      <c r="I28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="18"/>
-      <c r="B29" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="F29" s="32"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
+      <c r="A29" s="0"/>
+      <c r="B29" s="0"/>
+      <c r="C29" s="0"/>
+      <c r="D29" s="0"/>
+      <c r="E29" s="0"/>
+      <c r="F29" s="0"/>
+      <c r="G29" s="0"/>
+      <c r="H29" s="0"/>
+      <c r="I29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="18"/>
@@ -10639,9 +10550,9 @@
   <dimension ref="A1:EZ900"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+      <selection pane="bottomLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10841,13 +10752,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>14</v>
@@ -10883,7 +10794,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -10931,16 +10842,16 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="21" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
       <c r="H8" s="21" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -10959,186 +10870,150 @@
     <row r="10" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="18"/>
       <c r="B10" s="23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="25" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H10" s="26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I10" s="26"/>
       <c r="J10" s="26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
-      <c r="F11" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="F11" s="34"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="32"/>
       <c r="I11" s="32"/>
-      <c r="J11" s="32" t="s">
-        <v>95</v>
-      </c>
+      <c r="J11" s="32"/>
     </row>
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
-      <c r="F12" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="F12" s="34"/>
+      <c r="G12" s="33"/>
       <c r="H12" s="32"/>
       <c r="I12" s="32"/>
-      <c r="J12" s="32" t="s">
-        <v>95</v>
-      </c>
+      <c r="J12" s="32"/>
     </row>
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
-      <c r="F13" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="F13" s="35"/>
+      <c r="G13" s="33"/>
       <c r="H13" s="32"/>
       <c r="I13" s="32"/>
-      <c r="J13" s="32" t="s">
-        <v>95</v>
-      </c>
+      <c r="J13" s="32"/>
     </row>
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
-      <c r="F14" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="G14" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="F14" s="35"/>
+      <c r="G14" s="33"/>
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
-      <c r="J14" s="32" t="s">
-        <v>95</v>
-      </c>
+      <c r="J14" s="32"/>
     </row>
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
-      <c r="F15" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="F15" s="35"/>
+      <c r="G15" s="33"/>
       <c r="H15" s="32"/>
       <c r="I15" s="32"/>
-      <c r="J15" s="32" t="s">
-        <v>95</v>
-      </c>
+      <c r="J15" s="32"/>
     </row>
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
-      <c r="F16" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="G16" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="F16" s="35"/>
+      <c r="G16" s="33"/>
       <c r="H16" s="32"/>
       <c r="I16" s="32"/>
-      <c r="J16" s="32" t="s">
-        <v>95</v>
-      </c>
+      <c r="J16" s="32"/>
     </row>
     <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="33"/>
@@ -11149,14 +11024,14 @@
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="33"/>
@@ -11167,14 +11042,14 @@
     <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29"/>
       <c r="B19" s="30" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="33"/>
@@ -11185,14 +11060,14 @@
     <row r="20" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="30" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="33"/>
@@ -11202,14 +11077,14 @@
     </row>
     <row r="21" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="30" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="33"/>
@@ -11220,14 +11095,14 @@
     <row r="22" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="33"/>
@@ -11238,14 +11113,14 @@
     <row r="23" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="33"/>
@@ -11256,14 +11131,14 @@
     <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="30" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="33"/>

</xml_diff>

<commit_message>
Delete invalid tests from login and register tab. (#21)
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="117">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -111,6 +111,9 @@
   <si>
     <t xml:space="preserve">Not need valid email for registration. 
 Generate email account random string.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Playwright tool.</t>
   </si>
   <si>
     <t xml:space="preserve">ID</t>
@@ -242,55 +245,16 @@
     <t xml:space="preserve">001-14</t>
   </si>
   <si>
-    <t xml:space="preserve">Register with changed email.</t>
+    <t xml:space="preserve">Register user confirm password not matching password</t>
   </si>
   <si>
-    <t xml:space="preserve">User is registered with changed email.</t>
+    <t xml:space="preserve">User shouldn’t able to register without the Password and Confirm password fields are matching. Error message.</t>
   </si>
   <si>
     <t xml:space="preserve">001-15</t>
   </si>
   <si>
-    <t xml:space="preserve">Register with invalid changed mail.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User shouldn't able to register with invalid change mail. Error message.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">001-16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Register without select date of birth day.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User shouldn't able to register without selecting date of birth day. Error message.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">001-17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Register without select date of birth month.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User shouldn't able to register without selecting date of birth month. Error message.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">001-18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Register without select date of birth year.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should able to register without selecting date of birth year. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">001-19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Register without select.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should able to register without selecting date. Error message.</t>
+    <t xml:space="preserve">Register user Password field change after fill Password and Confirm password field.</t>
   </si>
   <si>
     <t xml:space="preserve">Buy product</t>
@@ -310,9 +274,6 @@
 Product not in the stock.</t>
   </si>
   <si>
-    <t xml:space="preserve">Cypress tool.</t>
-  </si>
-  <si>
     <t xml:space="preserve">002-01</t>
   </si>
   <si>
@@ -320,15 +281,6 @@
   </si>
   <si>
     <t xml:space="preserve">User should buy single product.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User can buy single product.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
   </si>
   <si>
     <t xml:space="preserve">002-02</t>
@@ -340,16 +292,10 @@
     <t xml:space="preserve">User should buy multiple products.</t>
   </si>
   <si>
-    <t xml:space="preserve">User can buy multiple product.</t>
-  </si>
-  <si>
     <t xml:space="preserve">002-03</t>
   </si>
   <si>
     <t xml:space="preserve">Buy multiple products different product.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User can buy multiple quantity from multiple product.</t>
   </si>
   <si>
     <t xml:space="preserve">002-04</t>
@@ -361,9 +307,6 @@
     <t xml:space="preserve">Cart should be empty.</t>
   </si>
   <si>
-    <t xml:space="preserve">Cart empty after user deleting item from it.</t>
-  </si>
-  <si>
     <t xml:space="preserve">002-05</t>
   </si>
   <si>
@@ -373,9 +316,6 @@
     <t xml:space="preserve">Only that product is missing which is removed.</t>
   </si>
   <si>
-    <t xml:space="preserve">Cart has one product after other product is deleted.</t>
-  </si>
-  <si>
     <t xml:space="preserve">002-06</t>
   </si>
   <si>
@@ -383,9 +323,6 @@
   </si>
   <si>
     <t xml:space="preserve">More product in the cart.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cart has increased the amount size.</t>
   </si>
   <si>
     <t xml:space="preserve">002-07</t>
@@ -1212,9 +1149,9 @@
   <dimension ref="A1:EZ899"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1514,7 +1451,9 @@
         <v>23</v>
       </c>
       <c r="G8" s="5"/>
-      <c r="H8" s="21"/>
+      <c r="H8" s="21" t="s">
+        <v>24</v>
+      </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -1532,42 +1471,42 @@
     <row r="10" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="18"/>
       <c r="B10" s="23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="25" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H10" s="26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I10" s="26"/>
       <c r="J10" s="26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="33"/>
@@ -1578,14 +1517,14 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F12" s="32"/>
       <c r="G12" s="33"/>
@@ -1596,14 +1535,14 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F13" s="32"/>
       <c r="G13" s="33"/>
@@ -1614,14 +1553,14 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="33"/>
@@ -1632,14 +1571,14 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F15" s="32"/>
       <c r="G15" s="33"/>
@@ -1650,14 +1589,14 @@
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F16" s="32"/>
       <c r="G16" s="33"/>
@@ -1668,14 +1607,14 @@
     <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="33"/>
@@ -1686,14 +1625,14 @@
     <row r="18" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F18" s="32"/>
       <c r="G18" s="33"/>
@@ -1704,38 +1643,38 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
     </row>
     <row r="20" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -1743,14 +1682,14 @@
     <row r="21" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="33"/>
@@ -1761,14 +1700,14 @@
     <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="33"/>
@@ -1779,14 +1718,14 @@
     <row r="23" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="33"/>
@@ -1794,17 +1733,17 @@
       <c r="I23" s="32"/>
       <c r="J23" s="32"/>
     </row>
-    <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="18"/>
+    <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0"/>
       <c r="B24" s="30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="33"/>
@@ -1812,17 +1751,17 @@
       <c r="I24" s="32"/>
       <c r="J24" s="32"/>
     </row>
-    <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="18"/>
+    <row r="25" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0"/>
       <c r="B25" s="30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="33"/>
@@ -1831,76 +1770,48 @@
       <c r="J25" s="32"/>
     </row>
     <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="18"/>
-      <c r="B26" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="32"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="32"/>
+      <c r="A26" s="0"/>
+      <c r="B26" s="0"/>
+      <c r="C26" s="0"/>
+      <c r="D26" s="0"/>
+      <c r="E26" s="0"/>
+      <c r="F26" s="0"/>
+      <c r="G26" s="0"/>
+      <c r="H26" s="0"/>
+      <c r="I26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="18"/>
-      <c r="B27" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="F27" s="32"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
+      <c r="A27" s="0"/>
+      <c r="B27" s="0"/>
+      <c r="C27" s="0"/>
+      <c r="D27" s="0"/>
+      <c r="E27" s="0"/>
+      <c r="F27" s="0"/>
+      <c r="G27" s="0"/>
+      <c r="H27" s="0"/>
+      <c r="I27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="18"/>
-      <c r="B28" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="A28" s="0"/>
+      <c r="B28" s="0"/>
+      <c r="C28" s="0"/>
+      <c r="D28" s="0"/>
+      <c r="E28" s="0"/>
+      <c r="F28" s="0"/>
+      <c r="G28" s="0"/>
+      <c r="H28" s="0"/>
+      <c r="I28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="18"/>
-      <c r="B29" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="F29" s="32"/>
-      <c r="G29" s="33"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
+      <c r="A29" s="0"/>
+      <c r="B29" s="0"/>
+      <c r="C29" s="0"/>
+      <c r="D29" s="0"/>
+      <c r="E29" s="0"/>
+      <c r="F29" s="0"/>
+      <c r="G29" s="0"/>
+      <c r="H29" s="0"/>
+      <c r="I29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="18"/>
@@ -10639,9 +10550,9 @@
   <dimension ref="A1:EZ900"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+      <selection pane="bottomLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10841,13 +10752,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>14</v>
@@ -10883,7 +10794,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -10931,16 +10842,16 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="21" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
       <c r="H8" s="21" t="s">
-        <v>89</v>
+        <v>24</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -10959,186 +10870,150 @@
     <row r="10" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="18"/>
       <c r="B10" s="23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D10" s="25" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H10" s="26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I10" s="26"/>
       <c r="J10" s="26" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
-      <c r="F11" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="F11" s="34"/>
+      <c r="G11" s="33"/>
       <c r="H11" s="32"/>
       <c r="I11" s="32"/>
-      <c r="J11" s="32" t="s">
-        <v>95</v>
-      </c>
+      <c r="J11" s="32"/>
     </row>
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
-      <c r="F12" s="34" t="s">
-        <v>99</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="F12" s="34"/>
+      <c r="G12" s="33"/>
       <c r="H12" s="32"/>
       <c r="I12" s="32"/>
-      <c r="J12" s="32" t="s">
-        <v>95</v>
-      </c>
+      <c r="J12" s="32"/>
     </row>
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
-      <c r="F13" s="35" t="s">
-        <v>102</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="F13" s="35"/>
+      <c r="G13" s="33"/>
       <c r="H13" s="32"/>
       <c r="I13" s="32"/>
-      <c r="J13" s="32" t="s">
-        <v>95</v>
-      </c>
+      <c r="J13" s="32"/>
     </row>
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
-      <c r="F14" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="G14" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="F14" s="35"/>
+      <c r="G14" s="33"/>
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
-      <c r="J14" s="32" t="s">
-        <v>95</v>
-      </c>
+      <c r="J14" s="32"/>
     </row>
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
-      <c r="F15" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="G15" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="F15" s="35"/>
+      <c r="G15" s="33"/>
       <c r="H15" s="32"/>
       <c r="I15" s="32"/>
-      <c r="J15" s="32" t="s">
-        <v>95</v>
-      </c>
+      <c r="J15" s="32"/>
     </row>
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
-      <c r="F16" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="G16" s="33" t="s">
-        <v>94</v>
-      </c>
+      <c r="F16" s="35"/>
+      <c r="G16" s="33"/>
       <c r="H16" s="32"/>
       <c r="I16" s="32"/>
-      <c r="J16" s="32" t="s">
-        <v>95</v>
-      </c>
+      <c r="J16" s="32"/>
     </row>
     <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="33"/>
@@ -11149,14 +11024,14 @@
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="33"/>
@@ -11167,14 +11042,14 @@
     <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29"/>
       <c r="B19" s="30" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="33"/>
@@ -11185,14 +11060,14 @@
     <row r="20" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="30" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="33"/>
@@ -11202,14 +11077,14 @@
     </row>
     <row r="21" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="30" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="33"/>
@@ -11220,14 +11095,14 @@
     <row r="22" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="33"/>
@@ -11238,14 +11113,14 @@
     <row r="23" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="33"/>
@@ -11256,14 +11131,14 @@
     <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="30" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="33"/>

</xml_diff>

<commit_message>
Add logout testcase. Delete invalid testcases from Buy products tab.
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Buy product" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'Buy product'!$B$1:$H$18</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'Buy product'!$B$1:$H$17</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Login and register'!$B$1:$H$18</definedName>
     <definedName function="false" hidden="false" name="_ITEM1" vbProcedure="false">'login and register'!#ref!</definedName>
     <definedName function="false" hidden="false" name="_ITEM2" vbProcedure="false">'login and register'!#ref!</definedName>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="105">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -257,6 +257,15 @@
     <t xml:space="preserve">Register user Password field change after fill Password and Confirm password field.</t>
   </si>
   <si>
+    <t xml:space="preserve">001-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logout from the webshop.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User able to logout from the webshop.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Buy product</t>
   </si>
   <si>
@@ -325,15 +334,6 @@
     <t xml:space="preserve">More product in the cart.</t>
   </si>
   <si>
-    <t xml:space="preserve">002-07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add more product to the cart what is in the stock.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User shouldn't able to add more product.</t>
-  </si>
-  <si>
     <t xml:space="preserve">002-08</t>
   </si>
   <si>
@@ -355,43 +355,7 @@
     <t xml:space="preserve">Try buy product without log in.</t>
   </si>
   <si>
-    <t xml:space="preserve">User shouldn't able to buy without sign in.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">002-11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Try input invalid address at the checkout.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User shouldn't able to buy with invalid address.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">002-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Try buy product without address.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User shouldn't able to buy without address.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">002-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Try buy without shipping option.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User shouldn't able to buy without shipping option.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">002-14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Try buy without giving payment option. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">User shouldn't able to buy without payment option.</t>
+    <t xml:space="preserve">User should able to buy without sign in. Can buy as a guest.</t>
   </si>
 </sst>
 </file>
@@ -1149,9 +1113,9 @@
   <dimension ref="A1:EZ899"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
+      <selection pane="bottomLeft" activeCell="L26" activeCellId="0" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1734,7 +1698,6 @@
       <c r="J23" s="32"/>
     </row>
     <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0"/>
       <c r="B24" s="30" t="s">
         <v>67</v>
       </c>
@@ -1752,7 +1715,6 @@
       <c r="J24" s="32"/>
     </row>
     <row r="25" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0"/>
       <c r="B25" s="30" t="s">
         <v>70</v>
       </c>
@@ -1769,50 +1731,25 @@
       <c r="I25" s="32"/>
       <c r="J25" s="32"/>
     </row>
-    <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0"/>
-      <c r="B26" s="0"/>
-      <c r="C26" s="0"/>
-      <c r="D26" s="0"/>
-      <c r="E26" s="0"/>
-      <c r="F26" s="0"/>
-      <c r="G26" s="0"/>
-      <c r="H26" s="0"/>
-      <c r="I26" s="0"/>
-    </row>
-    <row r="27" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0"/>
-      <c r="B27" s="0"/>
-      <c r="C27" s="0"/>
-      <c r="D27" s="0"/>
-      <c r="E27" s="0"/>
-      <c r="F27" s="0"/>
-      <c r="G27" s="0"/>
-      <c r="H27" s="0"/>
-      <c r="I27" s="0"/>
-    </row>
-    <row r="28" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0"/>
-      <c r="B28" s="0"/>
-      <c r="C28" s="0"/>
-      <c r="D28" s="0"/>
-      <c r="E28" s="0"/>
-      <c r="F28" s="0"/>
-      <c r="G28" s="0"/>
-      <c r="H28" s="0"/>
-      <c r="I28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0"/>
-      <c r="B29" s="0"/>
-      <c r="C29" s="0"/>
-      <c r="D29" s="0"/>
-      <c r="E29" s="0"/>
-      <c r="F29" s="0"/>
-      <c r="G29" s="0"/>
-      <c r="H29" s="0"/>
-      <c r="I29" s="0"/>
-    </row>
+    <row r="26" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="32"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+    </row>
+    <row r="27" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="18"/>
       <c r="B30" s="18"/>
@@ -10547,12 +10484,12 @@
     <tabColor rgb="FF8497B0"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:EZ900"/>
+  <dimension ref="A1:EZ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="E37" activeCellId="0" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10752,13 +10689,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>14</v>
@@ -10794,7 +10731,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -10842,11 +10779,11 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="21" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
@@ -10898,14 +10835,14 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
@@ -10916,14 +10853,14 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
@@ -10934,14 +10871,14 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
@@ -10952,14 +10889,14 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
@@ -10970,14 +10907,14 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
@@ -10988,14 +10925,14 @@
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
@@ -11003,17 +10940,17 @@
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>
     </row>
-    <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="33"/>
@@ -11024,10 +10961,10 @@
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
@@ -11039,17 +10976,17 @@
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
     </row>
-    <row r="19" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="29"/>
+    <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="33"/>
@@ -11057,94 +10994,55 @@
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
     </row>
-    <row r="20" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
-      <c r="B20" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="C20" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="F20" s="34"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-      <c r="J20" s="32"/>
-    </row>
-    <row r="21" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-    </row>
-    <row r="22" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
-      <c r="B22" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" s="12"/>
-      <c r="E22" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="F22" s="34"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="32"/>
-    </row>
-    <row r="23" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
-      <c r="B23" s="30" t="s">
-        <v>111</v>
-      </c>
-      <c r="C23" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="D23" s="12"/>
-      <c r="E23" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="F23" s="34"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="32"/>
-    </row>
-    <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
-      <c r="B24" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="C24" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="F24" s="34"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="32"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="32"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18"/>
@@ -19856,56 +19754,11 @@
       <c r="G895" s="18"/>
       <c r="H895" s="18"/>
     </row>
-    <row r="896" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A896" s="18"/>
-      <c r="B896" s="18"/>
-      <c r="C896" s="18"/>
-      <c r="D896" s="18"/>
-      <c r="E896" s="18"/>
-      <c r="F896" s="18"/>
-      <c r="G896" s="18"/>
-      <c r="H896" s="18"/>
-    </row>
-    <row r="897" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A897" s="18"/>
-      <c r="B897" s="18"/>
-      <c r="C897" s="18"/>
-      <c r="D897" s="18"/>
-      <c r="E897" s="18"/>
-      <c r="F897" s="18"/>
-      <c r="G897" s="18"/>
-      <c r="H897" s="18"/>
-    </row>
-    <row r="898" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A898" s="18"/>
-      <c r="B898" s="18"/>
-      <c r="C898" s="18"/>
-      <c r="D898" s="18"/>
-      <c r="E898" s="18"/>
-      <c r="F898" s="18"/>
-      <c r="G898" s="18"/>
-      <c r="H898" s="18"/>
-    </row>
-    <row r="899" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A899" s="18"/>
-      <c r="B899" s="18"/>
-      <c r="C899" s="18"/>
-      <c r="D899" s="18"/>
-      <c r="E899" s="18"/>
-      <c r="F899" s="18"/>
-      <c r="G899" s="18"/>
-      <c r="H899" s="18"/>
-    </row>
-    <row r="900" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A900" s="18"/>
-      <c r="B900" s="18"/>
-      <c r="C900" s="18"/>
-      <c r="D900" s="18"/>
-      <c r="E900" s="18"/>
-      <c r="F900" s="18"/>
-      <c r="G900" s="18"/>
-      <c r="H900" s="18"/>
-    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <conditionalFormatting sqref="D3">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="HIGH" dxfId="3">

</xml_diff>

<commit_message>
[WIP] Fix testcase naming. Paging issue and state fix.
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login and register" sheetId="1" state="visible" r:id="rId3"/>
@@ -148,7 +148,7 @@
     <t xml:space="preserve">001-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Login with valid email and password.</t>
+    <t xml:space="preserve">Login with valid email and password</t>
   </si>
   <si>
     <t xml:space="preserve">User can log in.</t>
@@ -157,7 +157,7 @@
     <t xml:space="preserve">001-02</t>
   </si>
   <si>
-    <t xml:space="preserve">Login with valid email and invalid password.</t>
+    <t xml:space="preserve">Login with valid email and invalid password</t>
   </si>
   <si>
     <t xml:space="preserve">User can't log in. Error message.</t>
@@ -166,19 +166,19 @@
     <t xml:space="preserve">001-03</t>
   </si>
   <si>
-    <t xml:space="preserve">Login with invalid email and valid password.</t>
+    <t xml:space="preserve">Login with invalid email and valid password</t>
   </si>
   <si>
     <t xml:space="preserve">001-04</t>
   </si>
   <si>
-    <t xml:space="preserve">Login with valid email and empty password.</t>
+    <t xml:space="preserve">Login with valid email and empty password</t>
   </si>
   <si>
     <t xml:space="preserve">001-05</t>
   </si>
   <si>
-    <t xml:space="preserve">Register user with valid email and password.</t>
+    <t xml:space="preserve">Register user with valid email and password</t>
   </si>
   <si>
     <t xml:space="preserve">User registered.</t>
@@ -187,7 +187,7 @@
     <t xml:space="preserve">001-06</t>
   </si>
   <si>
-    <t xml:space="preserve">Register user with invalid email and valid password.</t>
+    <t xml:space="preserve">Register user with invalid email and valid password</t>
   </si>
   <si>
     <t xml:space="preserve">User not registered. Error message.</t>
@@ -196,7 +196,7 @@
     <t xml:space="preserve">001-07</t>
   </si>
   <si>
-    <t xml:space="preserve">Register user with valid email and invalid password.</t>
+    <t xml:space="preserve">Register user with valid email and invalid password</t>
   </si>
   <si>
     <t xml:space="preserve">001-08</t>
@@ -226,7 +226,7 @@
     <t xml:space="preserve">001-11</t>
   </si>
   <si>
-    <t xml:space="preserve">Register user without selecting gender.</t>
+    <t xml:space="preserve">Register user without selecting gender</t>
   </si>
   <si>
     <t xml:space="preserve">User should able to register without selecting gender.</t>
@@ -235,7 +235,7 @@
     <t xml:space="preserve">001-12</t>
   </si>
   <si>
-    <t xml:space="preserve">Register user without input first name.</t>
+    <t xml:space="preserve">Register user without input first name</t>
   </si>
   <si>
     <t xml:space="preserve">User shouldn't able to register without input first name. Error message.</t>
@@ -244,7 +244,7 @@
     <t xml:space="preserve">001-13</t>
   </si>
   <si>
-    <t xml:space="preserve">Register user without input last name.</t>
+    <t xml:space="preserve">Register user without input last name</t>
   </si>
   <si>
     <t xml:space="preserve">User shouldn't able to register without input last name. Error message.</t>
@@ -262,13 +262,13 @@
     <t xml:space="preserve">001-15</t>
   </si>
   <si>
-    <t xml:space="preserve">Register user Password field change after fill Password and Confirm password field.</t>
+    <t xml:space="preserve">Register user Password field change after fill Password and Confirm password field</t>
   </si>
   <si>
     <t xml:space="preserve">001-16</t>
   </si>
   <si>
-    <t xml:space="preserve">Logout from the webshop.</t>
+    <t xml:space="preserve">Logout from the webshop</t>
   </si>
   <si>
     <t xml:space="preserve">User able to logout from the webshop.</t>
@@ -289,7 +289,7 @@
     <t xml:space="preserve">002-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Buy one product and checkout.</t>
+    <t xml:space="preserve">Buy one product and checkout</t>
   </si>
   <si>
     <t xml:space="preserve">User should buy single product.</t>
@@ -301,7 +301,7 @@
     <t xml:space="preserve">002-02</t>
   </si>
   <si>
-    <t xml:space="preserve">Buy multiple products same product.</t>
+    <t xml:space="preserve">Buy multiple products same product</t>
   </si>
   <si>
     <t xml:space="preserve">User should buy multiple products.</t>
@@ -310,13 +310,13 @@
     <t xml:space="preserve">002-03</t>
   </si>
   <si>
-    <t xml:space="preserve">Buy multiple products different product.</t>
+    <t xml:space="preserve">Buy multiple products different product</t>
   </si>
   <si>
     <t xml:space="preserve">002-04</t>
   </si>
   <si>
-    <t xml:space="preserve">Add product to the cart, remove from the cart.</t>
+    <t xml:space="preserve">Add product to the cart, remove from the cart</t>
   </si>
   <si>
     <t xml:space="preserve">Cart should be empty.</t>
@@ -325,7 +325,7 @@
     <t xml:space="preserve">002-05</t>
   </si>
   <si>
-    <t xml:space="preserve">Add multiple product to the cart, remove one product.</t>
+    <t xml:space="preserve">Add multiple product to the cart, remove one product</t>
   </si>
   <si>
     <t xml:space="preserve">Only that product is missing which is removed.</t>
@@ -334,7 +334,7 @@
     <t xml:space="preserve">002-06</t>
   </si>
   <si>
-    <t xml:space="preserve">Add one product to the cart, add more in the cart view.</t>
+    <t xml:space="preserve">Add one product to the cart, add more in the cart view</t>
   </si>
   <si>
     <t xml:space="preserve">More product in the cart.</t>
@@ -343,7 +343,7 @@
     <t xml:space="preserve">002-08</t>
   </si>
   <si>
-    <t xml:space="preserve">Add one product to the cart, try input minus number to the amount in the cart view.</t>
+    <t xml:space="preserve">Add one product to the cart, try input minus number to the amount in the cart view</t>
   </si>
   <si>
     <t xml:space="preserve">User shouldn't able to but minus or zero product.</t>
@@ -352,13 +352,13 @@
     <t xml:space="preserve">002-09</t>
   </si>
   <si>
-    <t xml:space="preserve">Add one product to the cart, try input zero to the amount in the cart view.</t>
+    <t xml:space="preserve">Add one product to the cart, try input zero to the amount in the cart view</t>
   </si>
   <si>
     <t xml:space="preserve">002-10</t>
   </si>
   <si>
-    <t xml:space="preserve">Try buy product without log in.</t>
+    <t xml:space="preserve">Try buy product without log in</t>
   </si>
   <si>
     <t xml:space="preserve">User should able to buy without sign in. Can buy as a guest.</t>
@@ -367,7 +367,7 @@
     <t xml:space="preserve">002-11</t>
   </si>
   <si>
-    <t xml:space="preserve">Add to cart from list view.</t>
+    <t xml:space="preserve">Add to cart from list view</t>
   </si>
   <si>
     <t xml:space="preserve">User should able to add product from list view.</t>
@@ -376,7 +376,7 @@
     <t xml:space="preserve">002-12</t>
   </si>
   <si>
-    <t xml:space="preserve">Add to cart from details view.</t>
+    <t xml:space="preserve">Add to cart from details view</t>
   </si>
   <si>
     <t xml:space="preserve">User should able to add product from detail view.</t>
@@ -394,7 +394,7 @@
     <t xml:space="preserve">002-14</t>
   </si>
   <si>
-    <t xml:space="preserve">Proceed buying without selecting shipping address with default address.</t>
+    <t xml:space="preserve">Proceed buying without selecting shipping address with default address</t>
   </si>
   <si>
     <t xml:space="preserve">User should able to proceed and the default address selected.</t>
@@ -421,7 +421,7 @@
     <t xml:space="preserve">002-17</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout with First name not filled.</t>
+    <t xml:space="preserve">Checkout with First name not filled</t>
   </si>
   <si>
     <t xml:space="preserve">User should not able to proceed with checkout and receiving an error message.</t>
@@ -430,43 +430,43 @@
     <t xml:space="preserve">002-18</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout with Last name not filled.</t>
+    <t xml:space="preserve">Checkout with Last name not filled</t>
   </si>
   <si>
     <t xml:space="preserve">002-19</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout with Email not filled.</t>
+    <t xml:space="preserve">Checkout with Email not filled</t>
   </si>
   <si>
     <t xml:space="preserve">002-20</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout with Country not selected.</t>
+    <t xml:space="preserve">Checkout with Country not selected</t>
   </si>
   <si>
     <t xml:space="preserve">002-21</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout with City not filled.</t>
+    <t xml:space="preserve">Checkout with City not filled</t>
   </si>
   <si>
     <t xml:space="preserve">002-22</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout with Address1 not filled.</t>
+    <t xml:space="preserve">Checkout with Address1 not filled</t>
   </si>
   <si>
     <t xml:space="preserve">002-23</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout with Address1 not filled but Address2 filled.</t>
+    <t xml:space="preserve">Checkout with Address1 not filled but Address2 filled</t>
   </si>
   <si>
     <t xml:space="preserve">002-24</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout with Phone number not filled.</t>
+    <t xml:space="preserve">Checkout with Phone number not filled</t>
   </si>
   <si>
     <t xml:space="preserve">002-25</t>
@@ -475,7 +475,7 @@
     <t xml:space="preserve">002-26</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout Shipping address to provided address.</t>
+    <t xml:space="preserve">Checkout Shipping address to provided address</t>
   </si>
   <si>
     <t xml:space="preserve">Provided address should be visible on the Shipping address page.</t>
@@ -484,7 +484,7 @@
     <t xml:space="preserve">002-27</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout Shipping address with In-Store Pickup selected.</t>
+    <t xml:space="preserve">Checkout Shipping address with In-Store Pickup selected</t>
   </si>
   <si>
     <t xml:space="preserve">Provided address should not be visible on the Shipping address page.</t>
@@ -523,7 +523,7 @@
     <t xml:space="preserve">003-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Click and email as a friend a product.</t>
+    <t xml:space="preserve">Click and email as a friend a product</t>
   </si>
   <si>
     <t xml:space="preserve">New window should appear with email and the link with the product is in the email.</t>
@@ -532,7 +532,7 @@
     <t xml:space="preserve">003-02</t>
   </si>
   <si>
-    <t xml:space="preserve">Add to compare multiple products to the compare list.</t>
+    <t xml:space="preserve">Add to compare multiple products to the compare list</t>
   </si>
   <si>
     <t xml:space="preserve">The user should able to compare multiple products by price and other attributes.</t>
@@ -541,7 +541,7 @@
     <t xml:space="preserve">003-03</t>
   </si>
   <si>
-    <t xml:space="preserve">Add coupon to the checkout process.</t>
+    <t xml:space="preserve">Add coupon to the checkout process</t>
   </si>
   <si>
     <t xml:space="preserve">Coupon is added to the payment and deduct from the final price.</t>
@@ -550,7 +550,7 @@
     <t xml:space="preserve">003-04</t>
   </si>
   <si>
-    <t xml:space="preserve">Add invalid coupon to the checkout process.</t>
+    <t xml:space="preserve">Add invalid coupon to the checkout process</t>
   </si>
   <si>
     <t xml:space="preserve">Invalid coupon is not accepted, the user cannot proceed. </t>
@@ -559,7 +559,7 @@
     <t xml:space="preserve">003-05</t>
   </si>
   <si>
-    <t xml:space="preserve">Add a gift card to the user and try pay with it.</t>
+    <t xml:space="preserve">Add a gift card to the user and try pay with it</t>
   </si>
   <si>
     <t xml:space="preserve">After the gift card added to the user it can select as payment method.</t>
@@ -568,7 +568,7 @@
     <t xml:space="preserve">003-06</t>
   </si>
   <si>
-    <t xml:space="preserve">Add a gift card to the user and try pay with it price is higher than the gift card balance.</t>
+    <t xml:space="preserve">Add a gift card to the user and try pay with it price is higher than the gift card balance</t>
   </si>
   <si>
     <t xml:space="preserve">After the gift card added to the user it can select as payment method. The payment is deducted the amount of the gift card.</t>
@@ -1329,9 +1329,9 @@
   <dimension ref="A1:EZ899"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L26" activeCellId="0" sqref="L26"/>
+      <selection pane="bottomLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10702,10 +10702,10 @@
   </sheetPr>
   <dimension ref="A1:EZ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20213,10 +20213,10 @@
   </sheetPr>
   <dimension ref="A1:EZ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Finish implementation. Add comments and formatting.
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Login and register" sheetId="1" state="visible" r:id="rId3"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="179">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -154,6 +154,9 @@
     <t xml:space="preserve">User can log in.</t>
   </si>
   <si>
+    <t xml:space="preserve">PASS</t>
+  </si>
+  <si>
     <t xml:space="preserve">001-02</t>
   </si>
   <si>
@@ -163,10 +166,19 @@
     <t xml:space="preserve">User can't log in. Error message.</t>
   </si>
   <si>
+    <t xml:space="preserve">User can’t log in. 
+Error messages: Login was unsuccessful. Please correct the errors and try again.
+The credentials provided are incorrect</t>
+  </si>
+  <si>
     <t xml:space="preserve">001-03</t>
   </si>
   <si>
     <t xml:space="preserve">Login with invalid email and valid password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can’ log in.
+Error message: Please enter a valid email address.</t>
   </si>
   <si>
     <t xml:space="preserve">001-04</t>
@@ -284,6 +296,9 @@
   </si>
   <si>
     <t xml:space="preserve">Buying single and multiple products from the webshop. Validate stock working can't buy empty stock. Validate can't checkout minus product. Validate can change amount of product after put in the cart.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No dependencies</t>
   </si>
   <si>
     <t xml:space="preserve">002-01</t>
@@ -1328,10 +1343,10 @@
   </sheetPr>
   <dimension ref="A1:EZ899"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1688,26 +1703,34 @@
       <c r="E11" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="33"/>
+      <c r="F11" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H11" s="32"/>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
     </row>
-    <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="33"/>
+        <v>38</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H12" s="32"/>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -1715,17 +1738,21 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33"/>
+        <v>38</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H13" s="32"/>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -1733,14 +1760,14 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="33"/>
@@ -1751,14 +1778,14 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F15" s="32"/>
       <c r="G15" s="33"/>
@@ -1769,14 +1796,14 @@
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F16" s="32"/>
       <c r="G16" s="33"/>
@@ -1787,14 +1814,14 @@
     <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="33"/>
@@ -1805,14 +1832,14 @@
     <row r="18" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F18" s="32"/>
       <c r="G18" s="33"/>
@@ -1823,38 +1850,38 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
     </row>
     <row r="20" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="30" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -1862,14 +1889,14 @@
     <row r="21" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="33"/>
@@ -1880,14 +1907,14 @@
     <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="33"/>
@@ -1898,14 +1925,14 @@
     <row r="23" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="33"/>
@@ -1915,14 +1942,14 @@
     </row>
     <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="30" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="33"/>
@@ -1932,14 +1959,14 @@
     </row>
     <row r="25" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="30" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="33"/>
@@ -1949,14 +1976,14 @@
     </row>
     <row r="26" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="30" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F26" s="32"/>
       <c r="G26" s="33"/>
@@ -10703,9 +10730,9 @@
   <dimension ref="A1:EZ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
+      <selection pane="bottomLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10905,13 +10932,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>29</v>
@@ -10947,7 +10974,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -10995,10 +11022,12 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="21"/>
+      <c r="E8" s="21" t="s">
+        <v>82</v>
+      </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
       <c r="H8" s="21" t="s">
@@ -11049,19 +11078,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -11069,19 +11098,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -11089,19 +11118,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -11109,19 +11138,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -11129,19 +11158,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -11149,19 +11178,19 @@
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>
@@ -11169,19 +11198,19 @@
     <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="33"/>
       <c r="H17" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
@@ -11189,19 +11218,19 @@
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="33"/>
       <c r="H18" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
@@ -11209,19 +11238,19 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
@@ -11229,19 +11258,19 @@
     <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="30" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -11249,19 +11278,19 @@
     <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="33"/>
       <c r="H21" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
@@ -11269,19 +11298,19 @@
     <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="33"/>
       <c r="H22" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I22" s="32"/>
       <c r="J22" s="32"/>
@@ -11289,19 +11318,19 @@
     <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="33"/>
       <c r="H23" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I23" s="32"/>
       <c r="J23" s="32"/>
@@ -11309,19 +11338,19 @@
     <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="30" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="33"/>
       <c r="H24" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I24" s="32"/>
       <c r="J24" s="32"/>
@@ -11329,14 +11358,14 @@
     <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18"/>
       <c r="B25" s="30" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F25" s="34"/>
       <c r="G25" s="33"/>
@@ -11347,19 +11376,19 @@
     <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18"/>
       <c r="B26" s="30" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F26" s="34"/>
       <c r="G26" s="33"/>
       <c r="H26" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I26" s="32"/>
       <c r="J26" s="32"/>
@@ -11367,19 +11396,19 @@
     <row r="27" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18"/>
       <c r="B27" s="30" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="33"/>
       <c r="H27" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I27" s="32"/>
       <c r="J27" s="32"/>
@@ -11387,19 +11416,19 @@
     <row r="28" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="18"/>
       <c r="B28" s="30" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F28" s="34"/>
       <c r="G28" s="33"/>
       <c r="H28" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I28" s="32"/>
       <c r="J28" s="32"/>
@@ -11407,19 +11436,19 @@
     <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="18"/>
       <c r="B29" s="30" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F29" s="34"/>
       <c r="G29" s="33"/>
       <c r="H29" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I29" s="32"/>
       <c r="J29" s="32"/>
@@ -11427,19 +11456,19 @@
     <row r="30" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="18"/>
       <c r="B30" s="30" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F30" s="34"/>
       <c r="G30" s="33"/>
       <c r="H30" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I30" s="32"/>
       <c r="J30" s="32"/>
@@ -11447,19 +11476,19 @@
     <row r="31" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="18"/>
       <c r="B31" s="30" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F31" s="34"/>
       <c r="G31" s="33"/>
       <c r="H31" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I31" s="32"/>
       <c r="J31" s="32"/>
@@ -11467,19 +11496,19 @@
     <row r="32" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="18"/>
       <c r="B32" s="30" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F32" s="34"/>
       <c r="G32" s="33"/>
       <c r="H32" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I32" s="32"/>
       <c r="J32" s="32"/>
@@ -11487,19 +11516,19 @@
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="18"/>
       <c r="B33" s="30" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="33"/>
       <c r="H33" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I33" s="32"/>
       <c r="J33" s="32"/>
@@ -11507,19 +11536,19 @@
     <row r="34" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18"/>
       <c r="B34" s="30" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="33"/>
       <c r="H34" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I34" s="32"/>
       <c r="J34" s="32"/>
@@ -11527,39 +11556,39 @@
     <row r="35" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="18"/>
       <c r="B35" s="30" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="32" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="33"/>
       <c r="H35" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I35" s="32"/>
       <c r="J35" s="32"/>
     </row>
-    <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="18"/>
       <c r="B36" s="30" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="32" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F36" s="34"/>
       <c r="G36" s="33"/>
       <c r="H36" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I36" s="32"/>
       <c r="J36" s="32"/>
@@ -11567,19 +11596,19 @@
     <row r="37" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18"/>
       <c r="B37" s="30" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="32" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="F37" s="34"/>
       <c r="G37" s="33"/>
       <c r="H37" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I37" s="32"/>
       <c r="J37" s="32"/>
@@ -11587,14 +11616,14 @@
     <row r="38" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="18"/>
       <c r="B38" s="30" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="32" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F38" s="34"/>
       <c r="G38" s="33"/>
@@ -20213,10 +20242,10 @@
   </sheetPr>
   <dimension ref="A1:EZ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20418,13 +20447,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>6</v>
@@ -20460,7 +20489,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -20508,10 +20537,12 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="21"/>
+      <c r="E8" s="21" t="s">
+        <v>82</v>
+      </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
       <c r="H8" s="21" t="s">
@@ -20562,19 +20593,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -20582,19 +20613,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -20602,19 +20633,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -20622,19 +20653,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -20642,19 +20673,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -20662,19 +20693,19 @@
     <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>

</xml_diff>

<commit_message>
28 add api support to open new issues (#165)
Currently only run on local https://github.com/RobertPecz/PlaywrightPetProject/issues/166 going to fix to execute both on local and Github.
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Login and register" sheetId="1" state="visible" r:id="rId3"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="179">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -148,37 +148,49 @@
     <t xml:space="preserve">001-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Login with valid email and password.</t>
+    <t xml:space="preserve">Login with valid email and password</t>
   </si>
   <si>
     <t xml:space="preserve">User can log in.</t>
   </si>
   <si>
+    <t xml:space="preserve">PASS</t>
+  </si>
+  <si>
     <t xml:space="preserve">001-02</t>
   </si>
   <si>
-    <t xml:space="preserve">Login with valid email and invalid password.</t>
+    <t xml:space="preserve">Login with valid email and invalid password</t>
   </si>
   <si>
     <t xml:space="preserve">User can't log in. Error message.</t>
   </si>
   <si>
+    <t xml:space="preserve">User can’t log in. 
+Error messages: Login was unsuccessful. Please correct the errors and try again.
+The credentials provided are incorrect</t>
+  </si>
+  <si>
     <t xml:space="preserve">001-03</t>
   </si>
   <si>
-    <t xml:space="preserve">Login with invalid email and valid password.</t>
+    <t xml:space="preserve">Login with invalid email and valid password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can’ log in.
+Error message: Please enter a valid email address.</t>
   </si>
   <si>
     <t xml:space="preserve">001-04</t>
   </si>
   <si>
-    <t xml:space="preserve">Login with valid email and empty password.</t>
+    <t xml:space="preserve">Login with valid email and empty password</t>
   </si>
   <si>
     <t xml:space="preserve">001-05</t>
   </si>
   <si>
-    <t xml:space="preserve">Register user with valid email and password.</t>
+    <t xml:space="preserve">Register user with valid email and password</t>
   </si>
   <si>
     <t xml:space="preserve">User registered.</t>
@@ -187,7 +199,7 @@
     <t xml:space="preserve">001-06</t>
   </si>
   <si>
-    <t xml:space="preserve">Register user with invalid email and valid password.</t>
+    <t xml:space="preserve">Register user with invalid email and valid password</t>
   </si>
   <si>
     <t xml:space="preserve">User not registered. Error message.</t>
@@ -196,7 +208,7 @@
     <t xml:space="preserve">001-07</t>
   </si>
   <si>
-    <t xml:space="preserve">Register user with valid email and invalid password.</t>
+    <t xml:space="preserve">Register user with valid email and invalid password</t>
   </si>
   <si>
     <t xml:space="preserve">001-08</t>
@@ -226,7 +238,7 @@
     <t xml:space="preserve">001-11</t>
   </si>
   <si>
-    <t xml:space="preserve">Register user without selecting gender.</t>
+    <t xml:space="preserve">Register user without selecting gender</t>
   </si>
   <si>
     <t xml:space="preserve">User should able to register without selecting gender.</t>
@@ -235,7 +247,7 @@
     <t xml:space="preserve">001-12</t>
   </si>
   <si>
-    <t xml:space="preserve">Register user without input first name.</t>
+    <t xml:space="preserve">Register user without input first name</t>
   </si>
   <si>
     <t xml:space="preserve">User shouldn't able to register without input first name. Error message.</t>
@@ -244,7 +256,7 @@
     <t xml:space="preserve">001-13</t>
   </si>
   <si>
-    <t xml:space="preserve">Register user without input last name.</t>
+    <t xml:space="preserve">Register user without input last name</t>
   </si>
   <si>
     <t xml:space="preserve">User shouldn't able to register without input last name. Error message.</t>
@@ -262,13 +274,13 @@
     <t xml:space="preserve">001-15</t>
   </si>
   <si>
-    <t xml:space="preserve">Register user Password field change after fill Password and Confirm password field.</t>
+    <t xml:space="preserve">Register user Password field change after fill Password and Confirm password field</t>
   </si>
   <si>
     <t xml:space="preserve">001-16</t>
   </si>
   <si>
-    <t xml:space="preserve">Logout from the webshop.</t>
+    <t xml:space="preserve">Logout from the webshop</t>
   </si>
   <si>
     <t xml:space="preserve">User able to logout from the webshop.</t>
@@ -286,10 +298,13 @@
     <t xml:space="preserve">Buying single and multiple products from the webshop. Validate stock working can't buy empty stock. Validate can't checkout minus product. Validate can change amount of product after put in the cart.</t>
   </si>
   <si>
+    <t xml:space="preserve">No dependencies</t>
+  </si>
+  <si>
     <t xml:space="preserve">002-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Buy one product and checkout.</t>
+    <t xml:space="preserve">Buy one product and checkout</t>
   </si>
   <si>
     <t xml:space="preserve">User should buy single product.</t>
@@ -301,7 +316,7 @@
     <t xml:space="preserve">002-02</t>
   </si>
   <si>
-    <t xml:space="preserve">Buy multiple products same product.</t>
+    <t xml:space="preserve">Buy multiple products same product</t>
   </si>
   <si>
     <t xml:space="preserve">User should buy multiple products.</t>
@@ -310,13 +325,13 @@
     <t xml:space="preserve">002-03</t>
   </si>
   <si>
-    <t xml:space="preserve">Buy multiple products different product.</t>
+    <t xml:space="preserve">Buy multiple products different product</t>
   </si>
   <si>
     <t xml:space="preserve">002-04</t>
   </si>
   <si>
-    <t xml:space="preserve">Add product to the cart, remove from the cart.</t>
+    <t xml:space="preserve">Add product to the cart, remove from the cart</t>
   </si>
   <si>
     <t xml:space="preserve">Cart should be empty.</t>
@@ -325,7 +340,7 @@
     <t xml:space="preserve">002-05</t>
   </si>
   <si>
-    <t xml:space="preserve">Add multiple product to the cart, remove one product.</t>
+    <t xml:space="preserve">Add multiple product to the cart, remove one product</t>
   </si>
   <si>
     <t xml:space="preserve">Only that product is missing which is removed.</t>
@@ -334,7 +349,7 @@
     <t xml:space="preserve">002-06</t>
   </si>
   <si>
-    <t xml:space="preserve">Add one product to the cart, add more in the cart view.</t>
+    <t xml:space="preserve">Add one product to the cart, add more in the cart view</t>
   </si>
   <si>
     <t xml:space="preserve">More product in the cart.</t>
@@ -343,7 +358,7 @@
     <t xml:space="preserve">002-08</t>
   </si>
   <si>
-    <t xml:space="preserve">Add one product to the cart, try input minus number to the amount in the cart view.</t>
+    <t xml:space="preserve">Add one product to the cart, try input minus number to the amount in the cart view</t>
   </si>
   <si>
     <t xml:space="preserve">User shouldn't able to but minus or zero product.</t>
@@ -352,13 +367,13 @@
     <t xml:space="preserve">002-09</t>
   </si>
   <si>
-    <t xml:space="preserve">Add one product to the cart, try input zero to the amount in the cart view.</t>
+    <t xml:space="preserve">Add one product to the cart, try input zero to the amount in the cart view</t>
   </si>
   <si>
     <t xml:space="preserve">002-10</t>
   </si>
   <si>
-    <t xml:space="preserve">Try buy product without log in.</t>
+    <t xml:space="preserve">Try buy product without log in</t>
   </si>
   <si>
     <t xml:space="preserve">User should able to buy without sign in. Can buy as a guest.</t>
@@ -367,7 +382,7 @@
     <t xml:space="preserve">002-11</t>
   </si>
   <si>
-    <t xml:space="preserve">Add to cart from list view.</t>
+    <t xml:space="preserve">Add to cart from list view</t>
   </si>
   <si>
     <t xml:space="preserve">User should able to add product from list view.</t>
@@ -376,7 +391,7 @@
     <t xml:space="preserve">002-12</t>
   </si>
   <si>
-    <t xml:space="preserve">Add to cart from details view.</t>
+    <t xml:space="preserve">Add to cart from details view</t>
   </si>
   <si>
     <t xml:space="preserve">User should able to add product from detail view.</t>
@@ -394,7 +409,7 @@
     <t xml:space="preserve">002-14</t>
   </si>
   <si>
-    <t xml:space="preserve">Proceed buying without selecting shipping address with default address.</t>
+    <t xml:space="preserve">Proceed buying without selecting shipping address with default address</t>
   </si>
   <si>
     <t xml:space="preserve">User should able to proceed and the default address selected.</t>
@@ -421,7 +436,7 @@
     <t xml:space="preserve">002-17</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout with First name not filled.</t>
+    <t xml:space="preserve">Checkout with First name not filled</t>
   </si>
   <si>
     <t xml:space="preserve">User should not able to proceed with checkout and receiving an error message.</t>
@@ -430,43 +445,43 @@
     <t xml:space="preserve">002-18</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout with Last name not filled.</t>
+    <t xml:space="preserve">Checkout with Last name not filled</t>
   </si>
   <si>
     <t xml:space="preserve">002-19</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout with Email not filled.</t>
+    <t xml:space="preserve">Checkout with Email not filled</t>
   </si>
   <si>
     <t xml:space="preserve">002-20</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout with Country not selected.</t>
+    <t xml:space="preserve">Checkout with Country not selected</t>
   </si>
   <si>
     <t xml:space="preserve">002-21</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout with City not filled.</t>
+    <t xml:space="preserve">Checkout with City not filled</t>
   </si>
   <si>
     <t xml:space="preserve">002-22</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout with Address1 not filled.</t>
+    <t xml:space="preserve">Checkout with Address1 not filled</t>
   </si>
   <si>
     <t xml:space="preserve">002-23</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout with Address1 not filled but Address2 filled.</t>
+    <t xml:space="preserve">Checkout with Address1 not filled but Address2 filled</t>
   </si>
   <si>
     <t xml:space="preserve">002-24</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout with Phone number not filled.</t>
+    <t xml:space="preserve">Checkout with Phone number not filled</t>
   </si>
   <si>
     <t xml:space="preserve">002-25</t>
@@ -475,7 +490,7 @@
     <t xml:space="preserve">002-26</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout Shipping address to provided address.</t>
+    <t xml:space="preserve">Checkout Shipping address to provided address</t>
   </si>
   <si>
     <t xml:space="preserve">Provided address should be visible on the Shipping address page.</t>
@@ -484,7 +499,7 @@
     <t xml:space="preserve">002-27</t>
   </si>
   <si>
-    <t xml:space="preserve">Checkout Shipping address with In-Store Pickup selected.</t>
+    <t xml:space="preserve">Checkout Shipping address with In-Store Pickup selected</t>
   </si>
   <si>
     <t xml:space="preserve">Provided address should not be visible on the Shipping address page.</t>
@@ -523,7 +538,7 @@
     <t xml:space="preserve">003-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Click and email as a friend a product.</t>
+    <t xml:space="preserve">Click and email as a friend a product</t>
   </si>
   <si>
     <t xml:space="preserve">New window should appear with email and the link with the product is in the email.</t>
@@ -532,7 +547,7 @@
     <t xml:space="preserve">003-02</t>
   </si>
   <si>
-    <t xml:space="preserve">Add to compare multiple products to the compare list.</t>
+    <t xml:space="preserve">Add to compare multiple products to the compare list</t>
   </si>
   <si>
     <t xml:space="preserve">The user should able to compare multiple products by price and other attributes.</t>
@@ -541,7 +556,7 @@
     <t xml:space="preserve">003-03</t>
   </si>
   <si>
-    <t xml:space="preserve">Add coupon to the checkout process.</t>
+    <t xml:space="preserve">Add coupon to the checkout process</t>
   </si>
   <si>
     <t xml:space="preserve">Coupon is added to the payment and deduct from the final price.</t>
@@ -550,7 +565,7 @@
     <t xml:space="preserve">003-04</t>
   </si>
   <si>
-    <t xml:space="preserve">Add invalid coupon to the checkout process.</t>
+    <t xml:space="preserve">Add invalid coupon to the checkout process</t>
   </si>
   <si>
     <t xml:space="preserve">Invalid coupon is not accepted, the user cannot proceed. </t>
@@ -559,7 +574,7 @@
     <t xml:space="preserve">003-05</t>
   </si>
   <si>
-    <t xml:space="preserve">Add a gift card to the user and try pay with it.</t>
+    <t xml:space="preserve">Add a gift card to the user and try pay with it</t>
   </si>
   <si>
     <t xml:space="preserve">After the gift card added to the user it can select as payment method.</t>
@@ -568,7 +583,7 @@
     <t xml:space="preserve">003-06</t>
   </si>
   <si>
-    <t xml:space="preserve">Add a gift card to the user and try pay with it price is higher than the gift card balance.</t>
+    <t xml:space="preserve">Add a gift card to the user and try pay with it price is higher than the gift card balance</t>
   </si>
   <si>
     <t xml:space="preserve">After the gift card added to the user it can select as payment method. The payment is deducted the amount of the gift card.</t>
@@ -1328,10 +1343,10 @@
   </sheetPr>
   <dimension ref="A1:EZ899"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L26" activeCellId="0" sqref="L26"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1688,26 +1703,34 @@
       <c r="E11" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="32"/>
-      <c r="G11" s="33"/>
+      <c r="F11" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H11" s="32"/>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
     </row>
-    <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="33"/>
+        <v>38</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H12" s="32"/>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -1715,17 +1738,21 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33"/>
+        <v>38</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H13" s="32"/>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -1733,14 +1760,14 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="33"/>
@@ -1751,14 +1778,14 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="F15" s="32"/>
       <c r="G15" s="33"/>
@@ -1769,14 +1796,14 @@
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F16" s="32"/>
       <c r="G16" s="33"/>
@@ -1787,14 +1814,14 @@
     <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="33"/>
@@ -1805,14 +1832,14 @@
     <row r="18" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F18" s="32"/>
       <c r="G18" s="33"/>
@@ -1823,38 +1850,38 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
     </row>
     <row r="20" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="30" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -1862,14 +1889,14 @@
     <row r="21" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="33"/>
@@ -1880,14 +1907,14 @@
     <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="33"/>
@@ -1898,14 +1925,14 @@
     <row r="23" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="33"/>
@@ -1915,14 +1942,14 @@
     </row>
     <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="30" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="33"/>
@@ -1932,14 +1959,14 @@
     </row>
     <row r="25" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="30" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="33"/>
@@ -1949,14 +1976,14 @@
     </row>
     <row r="26" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="30" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F26" s="32"/>
       <c r="G26" s="33"/>
@@ -10702,10 +10729,10 @@
   </sheetPr>
   <dimension ref="A1:EZ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10905,13 +10932,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>29</v>
@@ -10947,7 +10974,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -10995,10 +11022,12 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="21"/>
+      <c r="E8" s="21" t="s">
+        <v>82</v>
+      </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
       <c r="H8" s="21" t="s">
@@ -11049,19 +11078,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -11069,19 +11098,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -11089,19 +11118,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -11109,19 +11138,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -11129,19 +11158,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -11149,19 +11178,19 @@
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>
@@ -11169,19 +11198,19 @@
     <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="33"/>
       <c r="H17" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
@@ -11189,19 +11218,19 @@
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="33"/>
       <c r="H18" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
@@ -11209,19 +11238,19 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
@@ -11229,19 +11258,19 @@
     <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="30" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -11249,19 +11278,19 @@
     <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="33"/>
       <c r="H21" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
@@ -11269,19 +11298,19 @@
     <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="33"/>
       <c r="H22" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I22" s="32"/>
       <c r="J22" s="32"/>
@@ -11289,19 +11318,19 @@
     <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="33"/>
       <c r="H23" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I23" s="32"/>
       <c r="J23" s="32"/>
@@ -11309,19 +11338,19 @@
     <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="30" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="33"/>
       <c r="H24" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I24" s="32"/>
       <c r="J24" s="32"/>
@@ -11329,14 +11358,14 @@
     <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18"/>
       <c r="B25" s="30" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F25" s="34"/>
       <c r="G25" s="33"/>
@@ -11347,19 +11376,19 @@
     <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18"/>
       <c r="B26" s="30" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F26" s="34"/>
       <c r="G26" s="33"/>
       <c r="H26" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I26" s="32"/>
       <c r="J26" s="32"/>
@@ -11367,19 +11396,19 @@
     <row r="27" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18"/>
       <c r="B27" s="30" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="33"/>
       <c r="H27" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I27" s="32"/>
       <c r="J27" s="32"/>
@@ -11387,19 +11416,19 @@
     <row r="28" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="18"/>
       <c r="B28" s="30" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F28" s="34"/>
       <c r="G28" s="33"/>
       <c r="H28" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I28" s="32"/>
       <c r="J28" s="32"/>
@@ -11407,19 +11436,19 @@
     <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="18"/>
       <c r="B29" s="30" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F29" s="34"/>
       <c r="G29" s="33"/>
       <c r="H29" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I29" s="32"/>
       <c r="J29" s="32"/>
@@ -11427,19 +11456,19 @@
     <row r="30" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="18"/>
       <c r="B30" s="30" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F30" s="34"/>
       <c r="G30" s="33"/>
       <c r="H30" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I30" s="32"/>
       <c r="J30" s="32"/>
@@ -11447,19 +11476,19 @@
     <row r="31" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="18"/>
       <c r="B31" s="30" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F31" s="34"/>
       <c r="G31" s="33"/>
       <c r="H31" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I31" s="32"/>
       <c r="J31" s="32"/>
@@ -11467,19 +11496,19 @@
     <row r="32" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="18"/>
       <c r="B32" s="30" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F32" s="34"/>
       <c r="G32" s="33"/>
       <c r="H32" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I32" s="32"/>
       <c r="J32" s="32"/>
@@ -11487,19 +11516,19 @@
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="18"/>
       <c r="B33" s="30" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="33"/>
       <c r="H33" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I33" s="32"/>
       <c r="J33" s="32"/>
@@ -11507,19 +11536,19 @@
     <row r="34" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18"/>
       <c r="B34" s="30" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="32" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="33"/>
       <c r="H34" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I34" s="32"/>
       <c r="J34" s="32"/>
@@ -11527,39 +11556,39 @@
     <row r="35" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="18"/>
       <c r="B35" s="30" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="32" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="33"/>
       <c r="H35" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I35" s="32"/>
       <c r="J35" s="32"/>
     </row>
-    <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="18"/>
       <c r="B36" s="30" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="32" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="F36" s="34"/>
       <c r="G36" s="33"/>
       <c r="H36" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I36" s="32"/>
       <c r="J36" s="32"/>
@@ -11567,19 +11596,19 @@
     <row r="37" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18"/>
       <c r="B37" s="30" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="32" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="F37" s="34"/>
       <c r="G37" s="33"/>
       <c r="H37" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I37" s="32"/>
       <c r="J37" s="32"/>
@@ -11587,14 +11616,14 @@
     <row r="38" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="18"/>
       <c r="B38" s="30" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="32" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="F38" s="34"/>
       <c r="G38" s="33"/>
@@ -20214,9 +20243,9 @@
   <dimension ref="A1:EZ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20418,13 +20447,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>6</v>
@@ -20460,7 +20489,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -20508,10 +20537,12 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D8" s="5"/>
-      <c r="E8" s="21"/>
+      <c r="E8" s="21" t="s">
+        <v>82</v>
+      </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
       <c r="H8" s="21" t="s">
@@ -20562,19 +20593,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -20582,19 +20613,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -20602,19 +20633,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -20622,19 +20653,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -20642,19 +20673,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -20662,19 +20693,19 @@
     <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>

</xml_diff>

<commit_message>
[WIP] Implementing register user and populate data.
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="180">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -168,7 +168,7 @@
   <si>
     <t xml:space="preserve">User can’t log in. 
 Error messages: Login was unsuccessful. Please correct the errors and try again.
-The credentials provided are incorrect</t>
+The credentials provided are incorrect.</t>
   </si>
   <si>
     <t xml:space="preserve">001-03</t>
@@ -177,7 +177,7 @@
     <t xml:space="preserve">Login with invalid email and valid password</t>
   </si>
   <si>
-    <t xml:space="preserve">User can’ log in.
+    <t xml:space="preserve">User can’t log in.
 Error message: Please enter a valid email address.</t>
   </si>
   <si>
@@ -185,6 +185,10 @@
   </si>
   <si>
     <t xml:space="preserve">Login with valid email and empty password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can’t log in.
+Error message: The credentials provided are incorrect.</t>
   </si>
   <si>
     <t xml:space="preserve">001-05</t>
@@ -1343,10 +1347,10 @@
   </sheetPr>
   <dimension ref="A1:EZ899"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1769,7 +1773,9 @@
       <c r="E14" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="32"/>
+      <c r="F14" s="32" t="s">
+        <v>45</v>
+      </c>
       <c r="G14" s="33"/>
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
@@ -1778,14 +1784,14 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F15" s="32"/>
       <c r="G15" s="33"/>
@@ -1796,14 +1802,14 @@
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F16" s="32"/>
       <c r="G16" s="33"/>
@@ -1814,14 +1820,14 @@
     <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="33"/>
@@ -1832,14 +1838,14 @@
     <row r="18" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F18" s="32"/>
       <c r="G18" s="33"/>
@@ -1850,38 +1856,38 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
     </row>
     <row r="20" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="30" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -1889,14 +1895,14 @@
     <row r="21" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="33"/>
@@ -1907,14 +1913,14 @@
     <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="33"/>
@@ -1925,14 +1931,14 @@
     <row r="23" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="33"/>
@@ -1942,14 +1948,14 @@
     </row>
     <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="30" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="33"/>
@@ -1959,14 +1965,14 @@
     </row>
     <row r="25" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="33"/>
@@ -1976,14 +1982,14 @@
     </row>
     <row r="26" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="30" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F26" s="32"/>
       <c r="G26" s="33"/>
@@ -10932,13 +10938,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>29</v>
@@ -10974,7 +10980,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -11022,11 +11028,11 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="21" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
@@ -11078,19 +11084,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -11098,19 +11104,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -11118,19 +11124,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -11138,19 +11144,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -11158,19 +11164,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -11178,19 +11184,19 @@
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>
@@ -11198,19 +11204,19 @@
     <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="33"/>
       <c r="H17" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
@@ -11218,19 +11224,19 @@
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="33"/>
       <c r="H18" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
@@ -11238,19 +11244,19 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
@@ -11258,19 +11264,19 @@
     <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -11278,19 +11284,19 @@
     <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="33"/>
       <c r="H21" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
@@ -11298,19 +11304,19 @@
     <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="33"/>
       <c r="H22" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I22" s="32"/>
       <c r="J22" s="32"/>
@@ -11318,19 +11324,19 @@
     <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="33"/>
       <c r="H23" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I23" s="32"/>
       <c r="J23" s="32"/>
@@ -11338,19 +11344,19 @@
     <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="30" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="33"/>
       <c r="H24" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I24" s="32"/>
       <c r="J24" s="32"/>
@@ -11358,14 +11364,14 @@
     <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18"/>
       <c r="B25" s="30" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F25" s="34"/>
       <c r="G25" s="33"/>
@@ -11376,19 +11382,19 @@
     <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18"/>
       <c r="B26" s="30" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F26" s="34"/>
       <c r="G26" s="33"/>
       <c r="H26" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I26" s="32"/>
       <c r="J26" s="32"/>
@@ -11396,19 +11402,19 @@
     <row r="27" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18"/>
       <c r="B27" s="30" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="33"/>
       <c r="H27" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I27" s="32"/>
       <c r="J27" s="32"/>
@@ -11416,19 +11422,19 @@
     <row r="28" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="18"/>
       <c r="B28" s="30" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F28" s="34"/>
       <c r="G28" s="33"/>
       <c r="H28" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I28" s="32"/>
       <c r="J28" s="32"/>
@@ -11436,19 +11442,19 @@
     <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="18"/>
       <c r="B29" s="30" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F29" s="34"/>
       <c r="G29" s="33"/>
       <c r="H29" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I29" s="32"/>
       <c r="J29" s="32"/>
@@ -11456,19 +11462,19 @@
     <row r="30" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="18"/>
       <c r="B30" s="30" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F30" s="34"/>
       <c r="G30" s="33"/>
       <c r="H30" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I30" s="32"/>
       <c r="J30" s="32"/>
@@ -11476,19 +11482,19 @@
     <row r="31" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="18"/>
       <c r="B31" s="30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F31" s="34"/>
       <c r="G31" s="33"/>
       <c r="H31" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I31" s="32"/>
       <c r="J31" s="32"/>
@@ -11496,19 +11502,19 @@
     <row r="32" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="18"/>
       <c r="B32" s="30" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F32" s="34"/>
       <c r="G32" s="33"/>
       <c r="H32" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I32" s="32"/>
       <c r="J32" s="32"/>
@@ -11516,19 +11522,19 @@
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="18"/>
       <c r="B33" s="30" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="33"/>
       <c r="H33" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I33" s="32"/>
       <c r="J33" s="32"/>
@@ -11536,19 +11542,19 @@
     <row r="34" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18"/>
       <c r="B34" s="30" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="33"/>
       <c r="H34" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I34" s="32"/>
       <c r="J34" s="32"/>
@@ -11556,19 +11562,19 @@
     <row r="35" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="18"/>
       <c r="B35" s="30" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="32" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="33"/>
       <c r="H35" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I35" s="32"/>
       <c r="J35" s="32"/>
@@ -11576,19 +11582,19 @@
     <row r="36" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="18"/>
       <c r="B36" s="30" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="32" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F36" s="34"/>
       <c r="G36" s="33"/>
       <c r="H36" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I36" s="32"/>
       <c r="J36" s="32"/>
@@ -11596,19 +11602,19 @@
     <row r="37" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18"/>
       <c r="B37" s="30" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="32" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F37" s="34"/>
       <c r="G37" s="33"/>
       <c r="H37" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I37" s="32"/>
       <c r="J37" s="32"/>
@@ -11616,14 +11622,14 @@
     <row r="38" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="18"/>
       <c r="B38" s="30" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F38" s="34"/>
       <c r="G38" s="33"/>
@@ -20447,13 +20453,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>6</v>
@@ -20489,7 +20495,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -20537,11 +20543,11 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="21" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
@@ -20593,19 +20599,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -20613,19 +20619,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -20633,19 +20639,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -20653,19 +20659,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -20673,19 +20679,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -20693,19 +20699,19 @@
     <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>

</xml_diff>

<commit_message>
Finalize register user testcase
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="181">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t xml:space="preserve">User registered.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is registered.</t>
   </si>
   <si>
     <t xml:space="preserve">001-06</t>
@@ -1348,9 +1351,9 @@
   <dimension ref="A1:EZ899"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1776,7 +1779,9 @@
       <c r="F14" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="33"/>
+      <c r="G14" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -1793,8 +1798,12 @@
       <c r="E15" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="32"/>
-      <c r="G15" s="33"/>
+      <c r="F15" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H15" s="32"/>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -1802,14 +1811,14 @@
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F16" s="32"/>
       <c r="G16" s="33"/>
@@ -1820,14 +1829,14 @@
     <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="33"/>
@@ -1838,14 +1847,14 @@
     <row r="18" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F18" s="32"/>
       <c r="G18" s="33"/>
@@ -1856,38 +1865,38 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
     </row>
     <row r="20" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="30" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -1895,14 +1904,14 @@
     <row r="21" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="33"/>
@@ -1913,14 +1922,14 @@
     <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="33"/>
@@ -1931,14 +1940,14 @@
     <row r="23" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="33"/>
@@ -1948,14 +1957,14 @@
     </row>
     <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="30" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="33"/>
@@ -1965,14 +1974,14 @@
     </row>
     <row r="25" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="30" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="33"/>
@@ -1982,14 +1991,14 @@
     </row>
     <row r="26" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="30" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F26" s="32"/>
       <c r="G26" s="33"/>
@@ -10938,13 +10947,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>29</v>
@@ -10980,7 +10989,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -11028,11 +11037,11 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
@@ -11084,19 +11093,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -11104,19 +11113,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -11124,19 +11133,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -11144,19 +11153,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -11164,19 +11173,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -11184,19 +11193,19 @@
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>
@@ -11204,19 +11213,19 @@
     <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="33"/>
       <c r="H17" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
@@ -11224,19 +11233,19 @@
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="33"/>
       <c r="H18" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
@@ -11244,19 +11253,19 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
@@ -11264,19 +11273,19 @@
     <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -11284,19 +11293,19 @@
     <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="33"/>
       <c r="H21" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
@@ -11304,19 +11313,19 @@
     <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="33"/>
       <c r="H22" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I22" s="32"/>
       <c r="J22" s="32"/>
@@ -11324,19 +11333,19 @@
     <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="33"/>
       <c r="H23" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I23" s="32"/>
       <c r="J23" s="32"/>
@@ -11344,19 +11353,19 @@
     <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="30" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="33"/>
       <c r="H24" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I24" s="32"/>
       <c r="J24" s="32"/>
@@ -11364,14 +11373,14 @@
     <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18"/>
       <c r="B25" s="30" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F25" s="34"/>
       <c r="G25" s="33"/>
@@ -11382,19 +11391,19 @@
     <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18"/>
       <c r="B26" s="30" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F26" s="34"/>
       <c r="G26" s="33"/>
       <c r="H26" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I26" s="32"/>
       <c r="J26" s="32"/>
@@ -11402,19 +11411,19 @@
     <row r="27" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18"/>
       <c r="B27" s="30" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="33"/>
       <c r="H27" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I27" s="32"/>
       <c r="J27" s="32"/>
@@ -11422,19 +11431,19 @@
     <row r="28" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="18"/>
       <c r="B28" s="30" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F28" s="34"/>
       <c r="G28" s="33"/>
       <c r="H28" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I28" s="32"/>
       <c r="J28" s="32"/>
@@ -11442,19 +11451,19 @@
     <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="18"/>
       <c r="B29" s="30" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F29" s="34"/>
       <c r="G29" s="33"/>
       <c r="H29" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I29" s="32"/>
       <c r="J29" s="32"/>
@@ -11462,19 +11471,19 @@
     <row r="30" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="18"/>
       <c r="B30" s="30" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F30" s="34"/>
       <c r="G30" s="33"/>
       <c r="H30" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I30" s="32"/>
       <c r="J30" s="32"/>
@@ -11482,19 +11491,19 @@
     <row r="31" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="18"/>
       <c r="B31" s="30" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F31" s="34"/>
       <c r="G31" s="33"/>
       <c r="H31" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I31" s="32"/>
       <c r="J31" s="32"/>
@@ -11502,19 +11511,19 @@
     <row r="32" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="18"/>
       <c r="B32" s="30" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F32" s="34"/>
       <c r="G32" s="33"/>
       <c r="H32" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I32" s="32"/>
       <c r="J32" s="32"/>
@@ -11522,19 +11531,19 @@
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="18"/>
       <c r="B33" s="30" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="33"/>
       <c r="H33" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I33" s="32"/>
       <c r="J33" s="32"/>
@@ -11542,19 +11551,19 @@
     <row r="34" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18"/>
       <c r="B34" s="30" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="32" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="33"/>
       <c r="H34" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I34" s="32"/>
       <c r="J34" s="32"/>
@@ -11562,19 +11571,19 @@
     <row r="35" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="18"/>
       <c r="B35" s="30" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="32" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="33"/>
       <c r="H35" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I35" s="32"/>
       <c r="J35" s="32"/>
@@ -11582,19 +11591,19 @@
     <row r="36" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="18"/>
       <c r="B36" s="30" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="32" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F36" s="34"/>
       <c r="G36" s="33"/>
       <c r="H36" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I36" s="32"/>
       <c r="J36" s="32"/>
@@ -11602,19 +11611,19 @@
     <row r="37" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18"/>
       <c r="B37" s="30" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="32" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F37" s="34"/>
       <c r="G37" s="33"/>
       <c r="H37" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I37" s="32"/>
       <c r="J37" s="32"/>
@@ -11622,14 +11631,14 @@
     <row r="38" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="18"/>
       <c r="B38" s="30" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="32" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F38" s="34"/>
       <c r="G38" s="33"/>
@@ -20453,13 +20462,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>6</v>
@@ -20495,7 +20504,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -20543,11 +20552,11 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
@@ -20599,19 +20608,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -20619,19 +20628,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -20639,19 +20648,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -20659,19 +20668,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -20679,19 +20688,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -20699,19 +20708,19 @@
     <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>

</xml_diff>

<commit_message>
6 testcase register user with valid email and password (#171)
* [WIP] Implementing register user and populate data.

* Finalize register user testcase
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="181">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -168,7 +168,7 @@
   <si>
     <t xml:space="preserve">User can’t log in. 
 Error messages: Login was unsuccessful. Please correct the errors and try again.
-The credentials provided are incorrect</t>
+The credentials provided are incorrect.</t>
   </si>
   <si>
     <t xml:space="preserve">001-03</t>
@@ -177,7 +177,7 @@
     <t xml:space="preserve">Login with invalid email and valid password</t>
   </si>
   <si>
-    <t xml:space="preserve">User can’ log in.
+    <t xml:space="preserve">User can’t log in.
 Error message: Please enter a valid email address.</t>
   </si>
   <si>
@@ -187,6 +187,10 @@
     <t xml:space="preserve">Login with valid email and empty password</t>
   </si>
   <si>
+    <t xml:space="preserve">User can’t log in.
+Error message: The credentials provided are incorrect.</t>
+  </si>
+  <si>
     <t xml:space="preserve">001-05</t>
   </si>
   <si>
@@ -194,6 +198,9 @@
   </si>
   <si>
     <t xml:space="preserve">User registered.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is registered.</t>
   </si>
   <si>
     <t xml:space="preserve">001-06</t>
@@ -1343,10 +1350,10 @@
   </sheetPr>
   <dimension ref="A1:EZ899"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1769,8 +1776,12 @@
       <c r="E14" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
+      <c r="F14" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -1778,17 +1789,21 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="32"/>
-      <c r="G15" s="33"/>
+        <v>48</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H15" s="32"/>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -1796,14 +1811,14 @@
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F16" s="32"/>
       <c r="G16" s="33"/>
@@ -1814,14 +1829,14 @@
     <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="33"/>
@@ -1832,14 +1847,14 @@
     <row r="18" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F18" s="32"/>
       <c r="G18" s="33"/>
@@ -1850,38 +1865,38 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
     </row>
     <row r="20" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="30" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -1889,14 +1904,14 @@
     <row r="21" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="33"/>
@@ -1907,14 +1922,14 @@
     <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="33"/>
@@ -1925,14 +1940,14 @@
     <row r="23" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="33"/>
@@ -1942,14 +1957,14 @@
     </row>
     <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="30" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="33"/>
@@ -1959,14 +1974,14 @@
     </row>
     <row r="25" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="30" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="33"/>
@@ -1976,14 +1991,14 @@
     </row>
     <row r="26" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="30" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F26" s="32"/>
       <c r="G26" s="33"/>
@@ -10932,13 +10947,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>29</v>
@@ -10974,7 +10989,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -11022,11 +11037,11 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="21" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
@@ -11078,19 +11093,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -11098,19 +11113,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -11118,19 +11133,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -11138,19 +11153,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -11158,19 +11173,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -11178,19 +11193,19 @@
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>
@@ -11198,19 +11213,19 @@
     <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="33"/>
       <c r="H17" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
@@ -11218,19 +11233,19 @@
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="33"/>
       <c r="H18" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
@@ -11238,19 +11253,19 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
@@ -11258,19 +11273,19 @@
     <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="30" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -11278,19 +11293,19 @@
     <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="33"/>
       <c r="H21" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
@@ -11298,19 +11313,19 @@
     <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="33"/>
       <c r="H22" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I22" s="32"/>
       <c r="J22" s="32"/>
@@ -11318,19 +11333,19 @@
     <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="33"/>
       <c r="H23" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I23" s="32"/>
       <c r="J23" s="32"/>
@@ -11338,19 +11353,19 @@
     <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="30" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="33"/>
       <c r="H24" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I24" s="32"/>
       <c r="J24" s="32"/>
@@ -11358,14 +11373,14 @@
     <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18"/>
       <c r="B25" s="30" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F25" s="34"/>
       <c r="G25" s="33"/>
@@ -11376,19 +11391,19 @@
     <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18"/>
       <c r="B26" s="30" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F26" s="34"/>
       <c r="G26" s="33"/>
       <c r="H26" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I26" s="32"/>
       <c r="J26" s="32"/>
@@ -11396,19 +11411,19 @@
     <row r="27" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18"/>
       <c r="B27" s="30" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="32" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="33"/>
       <c r="H27" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I27" s="32"/>
       <c r="J27" s="32"/>
@@ -11416,19 +11431,19 @@
     <row r="28" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="18"/>
       <c r="B28" s="30" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="32" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F28" s="34"/>
       <c r="G28" s="33"/>
       <c r="H28" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I28" s="32"/>
       <c r="J28" s="32"/>
@@ -11436,19 +11451,19 @@
     <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="18"/>
       <c r="B29" s="30" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="32" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F29" s="34"/>
       <c r="G29" s="33"/>
       <c r="H29" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I29" s="32"/>
       <c r="J29" s="32"/>
@@ -11456,19 +11471,19 @@
     <row r="30" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="18"/>
       <c r="B30" s="30" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="32" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F30" s="34"/>
       <c r="G30" s="33"/>
       <c r="H30" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I30" s="32"/>
       <c r="J30" s="32"/>
@@ -11476,19 +11491,19 @@
     <row r="31" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="18"/>
       <c r="B31" s="30" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="32" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F31" s="34"/>
       <c r="G31" s="33"/>
       <c r="H31" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I31" s="32"/>
       <c r="J31" s="32"/>
@@ -11496,19 +11511,19 @@
     <row r="32" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="18"/>
       <c r="B32" s="30" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="32" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F32" s="34"/>
       <c r="G32" s="33"/>
       <c r="H32" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I32" s="32"/>
       <c r="J32" s="32"/>
@@ -11516,19 +11531,19 @@
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="18"/>
       <c r="B33" s="30" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="32" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="33"/>
       <c r="H33" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I33" s="32"/>
       <c r="J33" s="32"/>
@@ -11536,19 +11551,19 @@
     <row r="34" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18"/>
       <c r="B34" s="30" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="32" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="33"/>
       <c r="H34" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I34" s="32"/>
       <c r="J34" s="32"/>
@@ -11556,19 +11571,19 @@
     <row r="35" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="18"/>
       <c r="B35" s="30" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="32" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="33"/>
       <c r="H35" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I35" s="32"/>
       <c r="J35" s="32"/>
@@ -11576,19 +11591,19 @@
     <row r="36" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="18"/>
       <c r="B36" s="30" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="32" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="F36" s="34"/>
       <c r="G36" s="33"/>
       <c r="H36" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I36" s="32"/>
       <c r="J36" s="32"/>
@@ -11596,19 +11611,19 @@
     <row r="37" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18"/>
       <c r="B37" s="30" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="32" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F37" s="34"/>
       <c r="G37" s="33"/>
       <c r="H37" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I37" s="32"/>
       <c r="J37" s="32"/>
@@ -11616,14 +11631,14 @@
     <row r="38" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="18"/>
       <c r="B38" s="30" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="32" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F38" s="34"/>
       <c r="G38" s="33"/>
@@ -20447,13 +20462,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>6</v>
@@ -20489,7 +20504,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -20537,11 +20552,11 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="21" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
@@ -20593,19 +20608,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -20613,19 +20628,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -20633,19 +20648,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -20653,19 +20668,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -20673,19 +20688,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -20693,19 +20708,19 @@
     <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>

</xml_diff>

<commit_message>
Created invalid and empty password testcases
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="184">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -212,16 +212,29 @@
     <t xml:space="preserve">User not registered. Error message.</t>
   </si>
   <si>
+    <t xml:space="preserve">User can’t log in.
+Error message: Please enter a valid email address.
+Wrong email.</t>
+  </si>
+  <si>
     <t xml:space="preserve">001-07</t>
   </si>
   <si>
     <t xml:space="preserve">Register user with valid email and invalid password</t>
   </si>
   <si>
+    <t xml:space="preserve">User can’t log in.
+Error message: The password should have at least 6 characters.</t>
+  </si>
+  <si>
     <t xml:space="preserve">001-08</t>
   </si>
   <si>
     <t xml:space="preserve">Register user with valid email and empty password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can’t log in.
+Error message: Password is required.</t>
   </si>
   <si>
     <t xml:space="preserve">001-09</t>
@@ -1351,9 +1364,9 @@
   <dimension ref="A1:EZ899"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1808,7 +1821,7 @@
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
     </row>
-    <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
         <v>50</v>
@@ -1820,8 +1833,12 @@
       <c r="E16" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="33"/>
+      <c r="F16" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H16" s="32"/>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>
@@ -1829,17 +1846,21 @@
     <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
+      <c r="F17" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H17" s="32"/>
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
@@ -1847,17 +1868,21 @@
     <row r="18" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="33"/>
+      <c r="F18" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H18" s="32"/>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
@@ -1865,10 +1890,10 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
@@ -1877,17 +1902,17 @@
       <c r="F19" s="32"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
     </row>
     <row r="20" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="30" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
@@ -1896,7 +1921,7 @@
       <c r="F20" s="32"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -1904,14 +1929,14 @@
     <row r="21" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="33"/>
@@ -1922,14 +1947,14 @@
     <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="33"/>
@@ -1940,14 +1965,14 @@
     <row r="23" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="33"/>
@@ -1957,14 +1982,14 @@
     </row>
     <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="30" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="33"/>
@@ -1974,14 +1999,14 @@
     </row>
     <row r="25" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="30" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="33"/>
@@ -1991,14 +2016,14 @@
     </row>
     <row r="26" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="30" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F26" s="32"/>
       <c r="G26" s="33"/>
@@ -10947,13 +10972,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>29</v>
@@ -10989,7 +11014,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -11037,11 +11062,11 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="21" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
@@ -11093,19 +11118,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -11113,19 +11138,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -11133,19 +11158,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -11153,19 +11178,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -11173,19 +11198,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -11193,19 +11218,19 @@
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>
@@ -11213,19 +11238,19 @@
     <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="33"/>
       <c r="H17" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
@@ -11233,19 +11258,19 @@
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="33"/>
       <c r="H18" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
@@ -11253,19 +11278,19 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
@@ -11273,19 +11298,19 @@
     <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="30" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -11293,19 +11318,19 @@
     <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="33"/>
       <c r="H21" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
@@ -11313,19 +11338,19 @@
     <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="33"/>
       <c r="H22" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I22" s="32"/>
       <c r="J22" s="32"/>
@@ -11333,19 +11358,19 @@
     <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="33"/>
       <c r="H23" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I23" s="32"/>
       <c r="J23" s="32"/>
@@ -11353,19 +11378,19 @@
     <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="30" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="33"/>
       <c r="H24" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I24" s="32"/>
       <c r="J24" s="32"/>
@@ -11373,14 +11398,14 @@
     <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18"/>
       <c r="B25" s="30" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F25" s="34"/>
       <c r="G25" s="33"/>
@@ -11391,19 +11416,19 @@
     <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18"/>
       <c r="B26" s="30" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F26" s="34"/>
       <c r="G26" s="33"/>
       <c r="H26" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I26" s="32"/>
       <c r="J26" s="32"/>
@@ -11411,19 +11436,19 @@
     <row r="27" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18"/>
       <c r="B27" s="30" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="33"/>
       <c r="H27" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I27" s="32"/>
       <c r="J27" s="32"/>
@@ -11431,19 +11456,19 @@
     <row r="28" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="18"/>
       <c r="B28" s="30" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F28" s="34"/>
       <c r="G28" s="33"/>
       <c r="H28" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I28" s="32"/>
       <c r="J28" s="32"/>
@@ -11451,19 +11476,19 @@
     <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="18"/>
       <c r="B29" s="30" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F29" s="34"/>
       <c r="G29" s="33"/>
       <c r="H29" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I29" s="32"/>
       <c r="J29" s="32"/>
@@ -11471,19 +11496,19 @@
     <row r="30" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="18"/>
       <c r="B30" s="30" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F30" s="34"/>
       <c r="G30" s="33"/>
       <c r="H30" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I30" s="32"/>
       <c r="J30" s="32"/>
@@ -11491,19 +11516,19 @@
     <row r="31" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="18"/>
       <c r="B31" s="30" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F31" s="34"/>
       <c r="G31" s="33"/>
       <c r="H31" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I31" s="32"/>
       <c r="J31" s="32"/>
@@ -11511,19 +11536,19 @@
     <row r="32" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="18"/>
       <c r="B32" s="30" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F32" s="34"/>
       <c r="G32" s="33"/>
       <c r="H32" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I32" s="32"/>
       <c r="J32" s="32"/>
@@ -11531,19 +11556,19 @@
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="18"/>
       <c r="B33" s="30" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="33"/>
       <c r="H33" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I33" s="32"/>
       <c r="J33" s="32"/>
@@ -11551,19 +11576,19 @@
     <row r="34" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18"/>
       <c r="B34" s="30" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="33"/>
       <c r="H34" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I34" s="32"/>
       <c r="J34" s="32"/>
@@ -11571,19 +11596,19 @@
     <row r="35" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="18"/>
       <c r="B35" s="30" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="32" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="33"/>
       <c r="H35" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I35" s="32"/>
       <c r="J35" s="32"/>
@@ -11591,19 +11616,19 @@
     <row r="36" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="18"/>
       <c r="B36" s="30" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="32" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F36" s="34"/>
       <c r="G36" s="33"/>
       <c r="H36" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I36" s="32"/>
       <c r="J36" s="32"/>
@@ -11611,19 +11636,19 @@
     <row r="37" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18"/>
       <c r="B37" s="30" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="32" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F37" s="34"/>
       <c r="G37" s="33"/>
       <c r="H37" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I37" s="32"/>
       <c r="J37" s="32"/>
@@ -11631,14 +11656,14 @@
     <row r="38" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="18"/>
       <c r="B38" s="30" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="32" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F38" s="34"/>
       <c r="G38" s="33"/>
@@ -20462,13 +20487,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>6</v>
@@ -20504,7 +20529,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -20552,11 +20577,11 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="21" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
@@ -20608,19 +20633,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -20628,19 +20653,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -20648,19 +20673,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -20668,19 +20693,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -20688,19 +20713,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -20708,19 +20733,19 @@
     <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>

</xml_diff>

<commit_message>
Created invalid and empty password testcases (#173)
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="184">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -212,16 +212,29 @@
     <t xml:space="preserve">User not registered. Error message.</t>
   </si>
   <si>
+    <t xml:space="preserve">User can’t log in.
+Error message: Please enter a valid email address.
+Wrong email.</t>
+  </si>
+  <si>
     <t xml:space="preserve">001-07</t>
   </si>
   <si>
     <t xml:space="preserve">Register user with valid email and invalid password</t>
   </si>
   <si>
+    <t xml:space="preserve">User can’t log in.
+Error message: The password should have at least 6 characters.</t>
+  </si>
+  <si>
     <t xml:space="preserve">001-08</t>
   </si>
   <si>
     <t xml:space="preserve">Register user with valid email and empty password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can’t log in.
+Error message: Password is required.</t>
   </si>
   <si>
     <t xml:space="preserve">001-09</t>
@@ -1351,9 +1364,9 @@
   <dimension ref="A1:EZ899"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1808,7 +1821,7 @@
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
     </row>
-    <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
         <v>50</v>
@@ -1820,8 +1833,12 @@
       <c r="E16" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="33"/>
+      <c r="F16" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H16" s="32"/>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>
@@ -1829,17 +1846,21 @@
     <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
+      <c r="F17" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H17" s="32"/>
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
@@ -1847,17 +1868,21 @@
     <row r="18" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="33"/>
+      <c r="F18" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H18" s="32"/>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
@@ -1865,10 +1890,10 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
@@ -1877,17 +1902,17 @@
       <c r="F19" s="32"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
     </row>
     <row r="20" customFormat="false" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="30" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
@@ -1896,7 +1921,7 @@
       <c r="F20" s="32"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -1904,14 +1929,14 @@
     <row r="21" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="33"/>
@@ -1922,14 +1947,14 @@
     <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="33"/>
@@ -1940,14 +1965,14 @@
     <row r="23" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="33"/>
@@ -1957,14 +1982,14 @@
     </row>
     <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="30" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="33"/>
@@ -1974,14 +1999,14 @@
     </row>
     <row r="25" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="30" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="33"/>
@@ -1991,14 +2016,14 @@
     </row>
     <row r="26" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="30" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F26" s="32"/>
       <c r="G26" s="33"/>
@@ -10947,13 +10972,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>29</v>
@@ -10989,7 +11014,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -11037,11 +11062,11 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="21" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
@@ -11093,19 +11118,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -11113,19 +11138,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -11133,19 +11158,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -11153,19 +11178,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -11173,19 +11198,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -11193,19 +11218,19 @@
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>
@@ -11213,19 +11238,19 @@
     <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="33"/>
       <c r="H17" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
@@ -11233,19 +11258,19 @@
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="33"/>
       <c r="H18" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
@@ -11253,19 +11278,19 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
@@ -11273,19 +11298,19 @@
     <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="30" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -11293,19 +11318,19 @@
     <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="33"/>
       <c r="H21" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
@@ -11313,19 +11338,19 @@
     <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="33"/>
       <c r="H22" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I22" s="32"/>
       <c r="J22" s="32"/>
@@ -11333,19 +11358,19 @@
     <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="33"/>
       <c r="H23" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I23" s="32"/>
       <c r="J23" s="32"/>
@@ -11353,19 +11378,19 @@
     <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="30" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="33"/>
       <c r="H24" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I24" s="32"/>
       <c r="J24" s="32"/>
@@ -11373,14 +11398,14 @@
     <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18"/>
       <c r="B25" s="30" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F25" s="34"/>
       <c r="G25" s="33"/>
@@ -11391,19 +11416,19 @@
     <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18"/>
       <c r="B26" s="30" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F26" s="34"/>
       <c r="G26" s="33"/>
       <c r="H26" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I26" s="32"/>
       <c r="J26" s="32"/>
@@ -11411,19 +11436,19 @@
     <row r="27" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18"/>
       <c r="B27" s="30" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="33"/>
       <c r="H27" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I27" s="32"/>
       <c r="J27" s="32"/>
@@ -11431,19 +11456,19 @@
     <row r="28" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="18"/>
       <c r="B28" s="30" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F28" s="34"/>
       <c r="G28" s="33"/>
       <c r="H28" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I28" s="32"/>
       <c r="J28" s="32"/>
@@ -11451,19 +11476,19 @@
     <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="18"/>
       <c r="B29" s="30" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F29" s="34"/>
       <c r="G29" s="33"/>
       <c r="H29" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I29" s="32"/>
       <c r="J29" s="32"/>
@@ -11471,19 +11496,19 @@
     <row r="30" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="18"/>
       <c r="B30" s="30" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F30" s="34"/>
       <c r="G30" s="33"/>
       <c r="H30" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I30" s="32"/>
       <c r="J30" s="32"/>
@@ -11491,19 +11516,19 @@
     <row r="31" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="18"/>
       <c r="B31" s="30" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F31" s="34"/>
       <c r="G31" s="33"/>
       <c r="H31" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I31" s="32"/>
       <c r="J31" s="32"/>
@@ -11511,19 +11536,19 @@
     <row r="32" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="18"/>
       <c r="B32" s="30" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F32" s="34"/>
       <c r="G32" s="33"/>
       <c r="H32" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I32" s="32"/>
       <c r="J32" s="32"/>
@@ -11531,19 +11556,19 @@
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="18"/>
       <c r="B33" s="30" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="33"/>
       <c r="H33" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I33" s="32"/>
       <c r="J33" s="32"/>
@@ -11551,19 +11576,19 @@
     <row r="34" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18"/>
       <c r="B34" s="30" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="32" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="33"/>
       <c r="H34" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I34" s="32"/>
       <c r="J34" s="32"/>
@@ -11571,19 +11596,19 @@
     <row r="35" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="18"/>
       <c r="B35" s="30" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="32" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="33"/>
       <c r="H35" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I35" s="32"/>
       <c r="J35" s="32"/>
@@ -11591,19 +11616,19 @@
     <row r="36" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="18"/>
       <c r="B36" s="30" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="32" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F36" s="34"/>
       <c r="G36" s="33"/>
       <c r="H36" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I36" s="32"/>
       <c r="J36" s="32"/>
@@ -11611,19 +11636,19 @@
     <row r="37" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18"/>
       <c r="B37" s="30" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="32" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F37" s="34"/>
       <c r="G37" s="33"/>
       <c r="H37" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I37" s="32"/>
       <c r="J37" s="32"/>
@@ -11631,14 +11656,14 @@
     <row r="38" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="18"/>
       <c r="B38" s="30" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="32" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="F38" s="34"/>
       <c r="G38" s="33"/>
@@ -20462,13 +20487,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>6</v>
@@ -20504,7 +20529,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -20552,11 +20577,11 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="21" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
@@ -20608,19 +20633,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -20628,19 +20653,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -20648,19 +20673,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -20668,19 +20693,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -20688,19 +20713,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -20708,19 +20733,19 @@
     <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>

</xml_diff>

<commit_message>
Add testcase: Register user with empty email and valid password
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="184">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -243,7 +243,8 @@
     <t xml:space="preserve">Register user with empty email and valid password</t>
   </si>
   <si>
-    <t xml:space="preserve">Only if possible type password.</t>
+    <t xml:space="preserve">User can’t log in. 
+Error messages: Email is required.</t>
   </si>
   <si>
     <t xml:space="preserve">001-10</t>
@@ -1366,7 +1367,7 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+      <selection pane="bottomLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1899,11 +1900,13 @@
       <c r="E19" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="32" t="s">
+      <c r="F19" s="32" t="s">
         <v>62</v>
       </c>
+      <c r="G19" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="32"/>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
     </row>

</xml_diff>

<commit_message>
Add testcase: Register user with empty email and valid password (#193)
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="184">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -243,7 +243,8 @@
     <t xml:space="preserve">Register user with empty email and valid password</t>
   </si>
   <si>
-    <t xml:space="preserve">Only if possible type password.</t>
+    <t xml:space="preserve">User can’t log in. 
+Error messages: Email is required.</t>
   </si>
   <si>
     <t xml:space="preserve">001-10</t>
@@ -1366,7 +1367,7 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
+      <selection pane="bottomLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1899,11 +1900,13 @@
       <c r="E19" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="32" t="s">
+      <c r="F19" s="32" t="s">
         <v>62</v>
       </c>
+      <c r="G19" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="H19" s="32"/>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
     </row>

</xml_diff>

<commit_message>
Add testcase register user with already registered email (#196)
* Update gitignore

* Fix runtime issues

* Fix already registered email testcase
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="185">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -223,7 +223,7 @@
     <t xml:space="preserve">Register user with valid email and invalid password</t>
   </si>
   <si>
-    <t xml:space="preserve">User can’t log in.
+    <t xml:space="preserve">User can’t register.
 Error message: The password should have at least 6 characters.</t>
   </si>
   <si>
@@ -233,7 +233,7 @@
     <t xml:space="preserve">Register user with valid email and empty password</t>
   </si>
   <si>
-    <t xml:space="preserve">User can’t log in.
+    <t xml:space="preserve">User can’t register.
 Error message: Password is required.</t>
   </si>
   <si>
@@ -243,7 +243,7 @@
     <t xml:space="preserve">Register user with empty email and valid password</t>
   </si>
   <si>
-    <t xml:space="preserve">User can’t log in. 
+    <t xml:space="preserve">User can’t register. 
 Error messages: Email is required.</t>
   </si>
   <si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t xml:space="preserve">Register user with email what is already registered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User can’t register. Error message: The specified email already exists</t>
   </si>
   <si>
     <t xml:space="preserve">Use rob.pecz@gmail.com</t>
@@ -1367,7 +1370,7 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G20" activeCellId="0" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1921,10 +1924,12 @@
       <c r="E20" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="32"/>
+      <c r="F20" s="32" t="s">
+        <v>65</v>
+      </c>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -1932,14 +1937,14 @@
     <row r="21" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F21" s="32"/>
       <c r="G21" s="33"/>
@@ -1950,14 +1955,14 @@
     <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="33"/>
@@ -1968,14 +1973,14 @@
     <row r="23" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="33"/>
@@ -1985,14 +1990,14 @@
     </row>
     <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="30" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="33"/>
@@ -2002,14 +2007,14 @@
     </row>
     <row r="25" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="30" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="33"/>
@@ -2019,14 +2024,14 @@
     </row>
     <row r="26" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="30" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F26" s="32"/>
       <c r="G26" s="33"/>
@@ -10975,13 +10980,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>29</v>
@@ -11017,7 +11022,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -11065,11 +11070,11 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="21" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
@@ -11121,19 +11126,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -11141,19 +11146,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -11161,19 +11166,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -11181,19 +11186,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -11201,19 +11206,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -11221,19 +11226,19 @@
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>
@@ -11241,19 +11246,19 @@
     <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="33"/>
       <c r="H17" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
@@ -11261,19 +11266,19 @@
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="33"/>
       <c r="H18" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
@@ -11281,19 +11286,19 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
@@ -11301,19 +11306,19 @@
     <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="30" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -11321,19 +11326,19 @@
     <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="33"/>
       <c r="H21" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
@@ -11341,19 +11346,19 @@
     <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="33"/>
       <c r="H22" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I22" s="32"/>
       <c r="J22" s="32"/>
@@ -11361,19 +11366,19 @@
     <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="33"/>
       <c r="H23" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I23" s="32"/>
       <c r="J23" s="32"/>
@@ -11381,19 +11386,19 @@
     <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="30" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="33"/>
       <c r="H24" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I24" s="32"/>
       <c r="J24" s="32"/>
@@ -11401,14 +11406,14 @@
     <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18"/>
       <c r="B25" s="30" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F25" s="34"/>
       <c r="G25" s="33"/>
@@ -11419,19 +11424,19 @@
     <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18"/>
       <c r="B26" s="30" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F26" s="34"/>
       <c r="G26" s="33"/>
       <c r="H26" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I26" s="32"/>
       <c r="J26" s="32"/>
@@ -11439,19 +11444,19 @@
     <row r="27" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18"/>
       <c r="B27" s="30" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="32" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="33"/>
       <c r="H27" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I27" s="32"/>
       <c r="J27" s="32"/>
@@ -11459,19 +11464,19 @@
     <row r="28" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="18"/>
       <c r="B28" s="30" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="32" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F28" s="34"/>
       <c r="G28" s="33"/>
       <c r="H28" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I28" s="32"/>
       <c r="J28" s="32"/>
@@ -11479,19 +11484,19 @@
     <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="18"/>
       <c r="B29" s="30" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="32" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F29" s="34"/>
       <c r="G29" s="33"/>
       <c r="H29" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I29" s="32"/>
       <c r="J29" s="32"/>
@@ -11499,19 +11504,19 @@
     <row r="30" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="18"/>
       <c r="B30" s="30" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="32" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F30" s="34"/>
       <c r="G30" s="33"/>
       <c r="H30" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I30" s="32"/>
       <c r="J30" s="32"/>
@@ -11519,19 +11524,19 @@
     <row r="31" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="18"/>
       <c r="B31" s="30" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="32" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F31" s="34"/>
       <c r="G31" s="33"/>
       <c r="H31" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I31" s="32"/>
       <c r="J31" s="32"/>
@@ -11539,19 +11544,19 @@
     <row r="32" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="18"/>
       <c r="B32" s="30" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="32" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F32" s="34"/>
       <c r="G32" s="33"/>
       <c r="H32" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I32" s="32"/>
       <c r="J32" s="32"/>
@@ -11559,19 +11564,19 @@
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="18"/>
       <c r="B33" s="30" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="32" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="33"/>
       <c r="H33" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I33" s="32"/>
       <c r="J33" s="32"/>
@@ -11579,19 +11584,19 @@
     <row r="34" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18"/>
       <c r="B34" s="30" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="32" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="33"/>
       <c r="H34" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I34" s="32"/>
       <c r="J34" s="32"/>
@@ -11599,19 +11604,19 @@
     <row r="35" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="18"/>
       <c r="B35" s="30" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="32" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="33"/>
       <c r="H35" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I35" s="32"/>
       <c r="J35" s="32"/>
@@ -11619,19 +11624,19 @@
     <row r="36" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="18"/>
       <c r="B36" s="30" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="32" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F36" s="34"/>
       <c r="G36" s="33"/>
       <c r="H36" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I36" s="32"/>
       <c r="J36" s="32"/>
@@ -11639,19 +11644,19 @@
     <row r="37" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18"/>
       <c r="B37" s="30" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="32" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F37" s="34"/>
       <c r="G37" s="33"/>
       <c r="H37" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I37" s="32"/>
       <c r="J37" s="32"/>
@@ -11659,14 +11664,14 @@
     <row r="38" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="18"/>
       <c r="B38" s="30" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="32" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F38" s="34"/>
       <c r="G38" s="33"/>
@@ -20490,13 +20495,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>6</v>
@@ -20532,7 +20537,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -20580,11 +20585,11 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="21" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
@@ -20636,19 +20641,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -20656,19 +20661,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -20676,19 +20681,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -20696,19 +20701,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -20716,19 +20721,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -20736,19 +20741,19 @@
     <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>

</xml_diff>

<commit_message>
16 testcase register user without selecting gender (#199)
* Feature: Add eslint, prettier and husky

* Delete dotnotation

* Take out strict

* Fix husky pre-push

* Add lint script to package.json

* Extend eslint config

* Add tsconfig eslint. Fixes in eslint and tsconfig file

* Fix linting and compilation issues

* Fix linting issues
</commit_message>
<xml_diff>
--- a/testcases/automation_practice_testcases.xlsx
+++ b/testcases/automation_practice_testcases.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="186">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION TEMPLATE</t>
   </si>
@@ -253,7 +253,7 @@
     <t xml:space="preserve">Register user with email what is already registered</t>
   </si>
   <si>
-    <t xml:space="preserve">User can’t register. Error message: The specified email already exists</t>
+    <t xml:space="preserve">User can’t register. Error message: The specified email already exists.</t>
   </si>
   <si>
     <t xml:space="preserve">Use rob.pecz@gmail.com</t>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t xml:space="preserve">User should able to register without selecting gender.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User able to register without selecting gender.</t>
   </si>
   <si>
     <t xml:space="preserve">001-12</t>
@@ -1370,7 +1373,7 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1927,7 +1930,9 @@
       <c r="F20" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="G20" s="33"/>
+      <c r="G20" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H20" s="32" t="s">
         <v>66</v>
       </c>
@@ -1946,8 +1951,12 @@
       <c r="E21" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
+      <c r="F21" s="32" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" s="33" t="s">
+        <v>35</v>
+      </c>
       <c r="H21" s="32"/>
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
@@ -1955,14 +1964,14 @@
     <row r="22" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F22" s="32"/>
       <c r="G22" s="33"/>
@@ -1973,14 +1982,14 @@
     <row r="23" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="33"/>
@@ -1990,14 +1999,14 @@
     </row>
     <row r="24" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="30" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F24" s="32"/>
       <c r="G24" s="33"/>
@@ -2007,14 +2016,14 @@
     </row>
     <row r="25" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="30" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F25" s="32"/>
       <c r="G25" s="33"/>
@@ -2024,14 +2033,14 @@
     </row>
     <row r="26" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="30" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F26" s="32"/>
       <c r="G26" s="33"/>
@@ -10980,13 +10989,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>29</v>
@@ -11022,7 +11031,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -11070,11 +11079,11 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
@@ -11126,19 +11135,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -11146,19 +11155,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -11166,19 +11175,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -11186,19 +11195,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -11206,19 +11215,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -11226,19 +11235,19 @@
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>
@@ -11246,19 +11255,19 @@
     <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="29"/>
       <c r="B17" s="30" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="32" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F17" s="34"/>
       <c r="G17" s="33"/>
       <c r="H17" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
@@ -11266,19 +11275,19 @@
     <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="32" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F18" s="34"/>
       <c r="G18" s="33"/>
       <c r="H18" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
@@ -11286,19 +11295,19 @@
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="18"/>
       <c r="B19" s="30" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="32" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="F19" s="34"/>
       <c r="G19" s="33"/>
       <c r="H19" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
@@ -11306,19 +11315,19 @@
     <row r="20" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="18"/>
       <c r="B20" s="30" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="32" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F20" s="34"/>
       <c r="G20" s="33"/>
       <c r="H20" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
@@ -11326,19 +11335,19 @@
     <row r="21" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="18"/>
       <c r="B21" s="30" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="32" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F21" s="34"/>
       <c r="G21" s="33"/>
       <c r="H21" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
@@ -11346,19 +11355,19 @@
     <row r="22" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="18"/>
       <c r="B22" s="30" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="32" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F22" s="34"/>
       <c r="G22" s="33"/>
       <c r="H22" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I22" s="32"/>
       <c r="J22" s="32"/>
@@ -11366,19 +11375,19 @@
     <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="18"/>
       <c r="B23" s="30" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="32" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F23" s="34"/>
       <c r="G23" s="33"/>
       <c r="H23" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I23" s="32"/>
       <c r="J23" s="32"/>
@@ -11386,19 +11395,19 @@
     <row r="24" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="18"/>
       <c r="B24" s="30" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="32" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F24" s="34"/>
       <c r="G24" s="33"/>
       <c r="H24" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I24" s="32"/>
       <c r="J24" s="32"/>
@@ -11406,14 +11415,14 @@
     <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="18"/>
       <c r="B25" s="30" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="32" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F25" s="34"/>
       <c r="G25" s="33"/>
@@ -11424,19 +11433,19 @@
     <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="18"/>
       <c r="B26" s="30" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F26" s="34"/>
       <c r="G26" s="33"/>
       <c r="H26" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I26" s="32"/>
       <c r="J26" s="32"/>
@@ -11444,19 +11453,19 @@
     <row r="27" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="18"/>
       <c r="B27" s="30" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F27" s="34"/>
       <c r="G27" s="33"/>
       <c r="H27" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I27" s="32"/>
       <c r="J27" s="32"/>
@@ -11464,19 +11473,19 @@
     <row r="28" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="18"/>
       <c r="B28" s="30" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F28" s="34"/>
       <c r="G28" s="33"/>
       <c r="H28" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I28" s="32"/>
       <c r="J28" s="32"/>
@@ -11484,19 +11493,19 @@
     <row r="29" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="18"/>
       <c r="B29" s="30" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F29" s="34"/>
       <c r="G29" s="33"/>
       <c r="H29" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I29" s="32"/>
       <c r="J29" s="32"/>
@@ -11504,19 +11513,19 @@
     <row r="30" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="18"/>
       <c r="B30" s="30" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F30" s="34"/>
       <c r="G30" s="33"/>
       <c r="H30" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I30" s="32"/>
       <c r="J30" s="32"/>
@@ -11524,19 +11533,19 @@
     <row r="31" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="18"/>
       <c r="B31" s="30" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D31" s="12"/>
       <c r="E31" s="32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F31" s="34"/>
       <c r="G31" s="33"/>
       <c r="H31" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I31" s="32"/>
       <c r="J31" s="32"/>
@@ -11544,19 +11553,19 @@
     <row r="32" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="18"/>
       <c r="B32" s="30" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F32" s="34"/>
       <c r="G32" s="33"/>
       <c r="H32" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I32" s="32"/>
       <c r="J32" s="32"/>
@@ -11564,19 +11573,19 @@
     <row r="33" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="18"/>
       <c r="B33" s="30" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F33" s="34"/>
       <c r="G33" s="33"/>
       <c r="H33" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I33" s="32"/>
       <c r="J33" s="32"/>
@@ -11584,19 +11593,19 @@
     <row r="34" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="18"/>
       <c r="B34" s="30" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="32" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F34" s="34"/>
       <c r="G34" s="33"/>
       <c r="H34" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I34" s="32"/>
       <c r="J34" s="32"/>
@@ -11604,19 +11613,19 @@
     <row r="35" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="18"/>
       <c r="B35" s="30" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="32" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F35" s="34"/>
       <c r="G35" s="33"/>
       <c r="H35" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I35" s="32"/>
       <c r="J35" s="32"/>
@@ -11624,19 +11633,19 @@
     <row r="36" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="18"/>
       <c r="B36" s="30" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="32" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F36" s="34"/>
       <c r="G36" s="33"/>
       <c r="H36" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I36" s="32"/>
       <c r="J36" s="32"/>
@@ -11644,19 +11653,19 @@
     <row r="37" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="18"/>
       <c r="B37" s="30" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="32" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F37" s="34"/>
       <c r="G37" s="33"/>
       <c r="H37" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I37" s="32"/>
       <c r="J37" s="32"/>
@@ -11664,14 +11673,14 @@
     <row r="38" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="18"/>
       <c r="B38" s="30" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C38" s="31" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="32" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F38" s="34"/>
       <c r="G38" s="33"/>
@@ -20495,13 +20504,13 @@
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F3" s="8" t="n">
         <v>6</v>
@@ -20537,7 +20546,7 @@
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="20" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15" t="s">
@@ -20585,11 +20594,11 @@
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="20" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="5"/>
@@ -20641,19 +20650,19 @@
     <row r="11" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="29"/>
       <c r="B11" s="30" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="32" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F11" s="34"/>
       <c r="G11" s="33"/>
       <c r="H11" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I11" s="32"/>
       <c r="J11" s="32"/>
@@ -20661,19 +20670,19 @@
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="29"/>
       <c r="B12" s="30" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="32" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="33"/>
       <c r="H12" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
@@ -20681,19 +20690,19 @@
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="29"/>
       <c r="B13" s="30" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="32" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33"/>
       <c r="H13" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
@@ -20701,19 +20710,19 @@
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="29"/>
       <c r="B14" s="30" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="32" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F14" s="35"/>
       <c r="G14" s="33"/>
       <c r="H14" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
@@ -20721,19 +20730,19 @@
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
       <c r="B15" s="30" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="32" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F15" s="35"/>
       <c r="G15" s="33"/>
       <c r="H15" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
@@ -20741,19 +20750,19 @@
     <row r="16" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29"/>
       <c r="B16" s="30" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="32" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F16" s="35"/>
       <c r="G16" s="33"/>
       <c r="H16" s="32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>

</xml_diff>